<commit_message>
#17 #16 #4 #15 Done / Improoved
Planeinstellungen & Einstellungen fertiggestellt
</commit_message>
<xml_diff>
--- a/docs/ZeitplanIST.xlsx
+++ b/docs/ZeitplanIST.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mail\Code\pelan\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07A249EB-3E9C-4630-B9DB-0D7D865D418F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E353820-8084-461B-96BA-AD07C54837F6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="41235" yWindow="6060" windowWidth="20355" windowHeight="12765" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -684,7 +684,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -893,6 +893,39 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -960,18 +993,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1300,7 +1321,7 @@
   <dimension ref="A1:AR50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1316,198 +1337,198 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:44" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="95" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="84"/>
-      <c r="G1" s="84"/>
-      <c r="H1" s="84"/>
-      <c r="I1" s="84"/>
-      <c r="J1" s="84"/>
-      <c r="K1" s="84"/>
-      <c r="L1" s="84"/>
-      <c r="M1" s="84"/>
-      <c r="N1" s="84"/>
-      <c r="O1" s="84"/>
-      <c r="P1" s="84"/>
-      <c r="Q1" s="84"/>
-      <c r="R1" s="84"/>
-      <c r="S1" s="84"/>
-      <c r="T1" s="84"/>
-      <c r="U1" s="84"/>
-      <c r="V1" s="84"/>
-      <c r="W1" s="84"/>
-      <c r="X1" s="84"/>
-      <c r="Y1" s="84"/>
-      <c r="Z1" s="84"/>
-      <c r="AA1" s="84"/>
-      <c r="AB1" s="84"/>
-      <c r="AC1" s="84"/>
-      <c r="AD1" s="84"/>
-      <c r="AE1" s="84"/>
-      <c r="AF1" s="84"/>
-      <c r="AG1" s="84"/>
-      <c r="AH1" s="84"/>
-      <c r="AI1" s="84"/>
-      <c r="AJ1" s="84"/>
-      <c r="AK1" s="84"/>
-      <c r="AL1" s="84"/>
-      <c r="AM1" s="84"/>
-      <c r="AN1" s="84"/>
-      <c r="AO1" s="84"/>
-      <c r="AP1" s="84"/>
-      <c r="AQ1" s="84"/>
-      <c r="AR1" s="84"/>
+      <c r="B1" s="95"/>
+      <c r="C1" s="95"/>
+      <c r="D1" s="95"/>
+      <c r="E1" s="95"/>
+      <c r="F1" s="95"/>
+      <c r="G1" s="95"/>
+      <c r="H1" s="95"/>
+      <c r="I1" s="95"/>
+      <c r="J1" s="95"/>
+      <c r="K1" s="95"/>
+      <c r="L1" s="95"/>
+      <c r="M1" s="95"/>
+      <c r="N1" s="95"/>
+      <c r="O1" s="95"/>
+      <c r="P1" s="95"/>
+      <c r="Q1" s="95"/>
+      <c r="R1" s="95"/>
+      <c r="S1" s="95"/>
+      <c r="T1" s="95"/>
+      <c r="U1" s="95"/>
+      <c r="V1" s="95"/>
+      <c r="W1" s="95"/>
+      <c r="X1" s="95"/>
+      <c r="Y1" s="95"/>
+      <c r="Z1" s="95"/>
+      <c r="AA1" s="95"/>
+      <c r="AB1" s="95"/>
+      <c r="AC1" s="95"/>
+      <c r="AD1" s="95"/>
+      <c r="AE1" s="95"/>
+      <c r="AF1" s="95"/>
+      <c r="AG1" s="95"/>
+      <c r="AH1" s="95"/>
+      <c r="AI1" s="95"/>
+      <c r="AJ1" s="95"/>
+      <c r="AK1" s="95"/>
+      <c r="AL1" s="95"/>
+      <c r="AM1" s="95"/>
+      <c r="AN1" s="95"/>
+      <c r="AO1" s="95"/>
+      <c r="AP1" s="95"/>
+      <c r="AQ1" s="95"/>
+      <c r="AR1" s="95"/>
     </row>
     <row r="2" spans="1:44" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="81" t="s">
+      <c r="A2" s="92" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="82"/>
-      <c r="C2" s="73" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="75"/>
-      <c r="E2" s="73" t="s">
+      <c r="B2" s="93"/>
+      <c r="C2" s="84" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="86"/>
+      <c r="E2" s="84" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="74"/>
-      <c r="G2" s="74"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="73" t="s">
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="84" t="s">
         <v>38</v>
       </c>
-      <c r="J2" s="74"/>
-      <c r="K2" s="74"/>
-      <c r="L2" s="75"/>
-      <c r="M2" s="73" t="s">
+      <c r="J2" s="85"/>
+      <c r="K2" s="85"/>
+      <c r="L2" s="86"/>
+      <c r="M2" s="84" t="s">
         <v>39</v>
       </c>
-      <c r="N2" s="74"/>
-      <c r="O2" s="74"/>
-      <c r="P2" s="75"/>
-      <c r="Q2" s="73" t="s">
+      <c r="N2" s="85"/>
+      <c r="O2" s="85"/>
+      <c r="P2" s="86"/>
+      <c r="Q2" s="84" t="s">
         <v>40</v>
       </c>
-      <c r="R2" s="74"/>
-      <c r="S2" s="74"/>
-      <c r="T2" s="75"/>
-      <c r="U2" s="73" t="s">
+      <c r="R2" s="85"/>
+      <c r="S2" s="85"/>
+      <c r="T2" s="86"/>
+      <c r="U2" s="84" t="s">
         <v>41</v>
       </c>
-      <c r="V2" s="74"/>
-      <c r="W2" s="74"/>
-      <c r="X2" s="75"/>
-      <c r="Y2" s="73" t="s">
+      <c r="V2" s="85"/>
+      <c r="W2" s="85"/>
+      <c r="X2" s="86"/>
+      <c r="Y2" s="84" t="s">
         <v>42</v>
       </c>
-      <c r="Z2" s="74"/>
-      <c r="AA2" s="74"/>
-      <c r="AB2" s="75"/>
-      <c r="AC2" s="73" t="s">
+      <c r="Z2" s="85"/>
+      <c r="AA2" s="85"/>
+      <c r="AB2" s="86"/>
+      <c r="AC2" s="84" t="s">
         <v>43</v>
       </c>
-      <c r="AD2" s="74"/>
-      <c r="AE2" s="74"/>
-      <c r="AF2" s="75"/>
-      <c r="AG2" s="73" t="s">
+      <c r="AD2" s="85"/>
+      <c r="AE2" s="85"/>
+      <c r="AF2" s="86"/>
+      <c r="AG2" s="84" t="s">
         <v>44</v>
       </c>
-      <c r="AH2" s="74"/>
-      <c r="AI2" s="74"/>
-      <c r="AJ2" s="75"/>
-      <c r="AK2" s="73" t="s">
+      <c r="AH2" s="85"/>
+      <c r="AI2" s="85"/>
+      <c r="AJ2" s="86"/>
+      <c r="AK2" s="84" t="s">
         <v>45</v>
       </c>
-      <c r="AL2" s="74"/>
-      <c r="AM2" s="74"/>
-      <c r="AN2" s="75"/>
-      <c r="AO2" s="73" t="s">
+      <c r="AL2" s="85"/>
+      <c r="AM2" s="85"/>
+      <c r="AN2" s="86"/>
+      <c r="AO2" s="84" t="s">
         <v>46</v>
       </c>
-      <c r="AP2" s="74"/>
-      <c r="AQ2" s="74"/>
-      <c r="AR2" s="75"/>
+      <c r="AP2" s="85"/>
+      <c r="AQ2" s="85"/>
+      <c r="AR2" s="86"/>
     </row>
     <row r="3" spans="1:44" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="81"/>
-      <c r="B3" s="82"/>
-      <c r="C3" s="76"/>
-      <c r="D3" s="78"/>
-      <c r="E3" s="76" t="s">
+      <c r="A3" s="92"/>
+      <c r="B3" s="93"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="87" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="77"/>
-      <c r="G3" s="77"/>
-      <c r="H3" s="78"/>
-      <c r="I3" s="76" t="s">
+      <c r="F3" s="88"/>
+      <c r="G3" s="88"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="87" t="s">
         <v>29</v>
       </c>
-      <c r="J3" s="77"/>
-      <c r="K3" s="77"/>
-      <c r="L3" s="78"/>
-      <c r="M3" s="76" t="s">
+      <c r="J3" s="88"/>
+      <c r="K3" s="88"/>
+      <c r="L3" s="89"/>
+      <c r="M3" s="87" t="s">
         <v>30</v>
       </c>
-      <c r="N3" s="77"/>
-      <c r="O3" s="77"/>
-      <c r="P3" s="78"/>
-      <c r="Q3" s="76" t="s">
+      <c r="N3" s="88"/>
+      <c r="O3" s="88"/>
+      <c r="P3" s="89"/>
+      <c r="Q3" s="87" t="s">
         <v>31</v>
       </c>
-      <c r="R3" s="77"/>
-      <c r="S3" s="77"/>
-      <c r="T3" s="78"/>
-      <c r="U3" s="76" t="s">
+      <c r="R3" s="88"/>
+      <c r="S3" s="88"/>
+      <c r="T3" s="89"/>
+      <c r="U3" s="87" t="s">
         <v>32</v>
       </c>
-      <c r="V3" s="77"/>
-      <c r="W3" s="77"/>
-      <c r="X3" s="78"/>
-      <c r="Y3" s="76" t="s">
+      <c r="V3" s="88"/>
+      <c r="W3" s="88"/>
+      <c r="X3" s="89"/>
+      <c r="Y3" s="87" t="s">
         <v>33</v>
       </c>
-      <c r="Z3" s="77"/>
-      <c r="AA3" s="77"/>
-      <c r="AB3" s="78"/>
-      <c r="AC3" s="76" t="s">
+      <c r="Z3" s="88"/>
+      <c r="AA3" s="88"/>
+      <c r="AB3" s="89"/>
+      <c r="AC3" s="87" t="s">
         <v>34</v>
       </c>
-      <c r="AD3" s="77"/>
-      <c r="AE3" s="77"/>
-      <c r="AF3" s="78"/>
-      <c r="AG3" s="76" t="s">
+      <c r="AD3" s="88"/>
+      <c r="AE3" s="88"/>
+      <c r="AF3" s="89"/>
+      <c r="AG3" s="87" t="s">
         <v>35</v>
       </c>
-      <c r="AH3" s="77"/>
-      <c r="AI3" s="77"/>
-      <c r="AJ3" s="78"/>
-      <c r="AK3" s="76" t="s">
+      <c r="AH3" s="88"/>
+      <c r="AI3" s="88"/>
+      <c r="AJ3" s="89"/>
+      <c r="AK3" s="87" t="s">
         <v>36</v>
       </c>
-      <c r="AL3" s="77"/>
-      <c r="AM3" s="77"/>
-      <c r="AN3" s="78"/>
-      <c r="AO3" s="76" t="s">
+      <c r="AL3" s="88"/>
+      <c r="AM3" s="88"/>
+      <c r="AN3" s="89"/>
+      <c r="AO3" s="87" t="s">
         <v>37</v>
       </c>
-      <c r="AP3" s="77"/>
-      <c r="AQ3" s="77"/>
-      <c r="AR3" s="78"/>
+      <c r="AP3" s="88"/>
+      <c r="AQ3" s="88"/>
+      <c r="AR3" s="89"/>
     </row>
     <row r="4" spans="1:44" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="79" t="s">
+      <c r="A4" s="90" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="80"/>
-      <c r="C4" s="83" t="s">
+      <c r="B4" s="91"/>
+      <c r="C4" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="80"/>
+      <c r="D4" s="91"/>
       <c r="E4" s="45">
         <v>2</v>
       </c>
@@ -1630,10 +1651,10 @@
       </c>
     </row>
     <row r="5" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="72" t="s">
+      <c r="A5" s="83" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="70" t="s">
+      <c r="B5" s="81" t="s">
         <v>50</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -1684,13 +1705,13 @@
       <c r="AR5" s="22"/>
     </row>
     <row r="6" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="73"/>
-      <c r="B6" s="70"/>
+      <c r="A6" s="84"/>
+      <c r="B6" s="81"/>
       <c r="C6" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="58"/>
-      <c r="E6" s="93"/>
+      <c r="E6" s="70"/>
       <c r="F6" s="19"/>
       <c r="G6" s="19"/>
       <c r="H6" s="40"/>
@@ -1732,7 +1753,7 @@
       <c r="AR6" s="23"/>
     </row>
     <row r="7" spans="1:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="92" t="s">
+      <c r="A7" s="103" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="44"/>
@@ -1744,23 +1765,23 @@
         <v>34</v>
       </c>
       <c r="E7" s="44"/>
-      <c r="F7" s="90"/>
-      <c r="G7" s="90"/>
-      <c r="H7" s="90"/>
-      <c r="I7" s="90"/>
-      <c r="J7" s="90"/>
-      <c r="K7" s="90"/>
-      <c r="L7" s="90"/>
-      <c r="M7" s="90"/>
-      <c r="N7" s="90"/>
-      <c r="O7" s="90"/>
-      <c r="P7" s="90"/>
-      <c r="Q7" s="90"/>
-      <c r="R7" s="90"/>
-      <c r="S7" s="90"/>
-      <c r="T7" s="90"/>
-      <c r="U7" s="90"/>
-      <c r="V7" s="90"/>
+      <c r="F7" s="101"/>
+      <c r="G7" s="101"/>
+      <c r="H7" s="101"/>
+      <c r="I7" s="101"/>
+      <c r="J7" s="101"/>
+      <c r="K7" s="101"/>
+      <c r="L7" s="101"/>
+      <c r="M7" s="101"/>
+      <c r="N7" s="101"/>
+      <c r="O7" s="101"/>
+      <c r="P7" s="101"/>
+      <c r="Q7" s="101"/>
+      <c r="R7" s="101"/>
+      <c r="S7" s="101"/>
+      <c r="T7" s="101"/>
+      <c r="U7" s="101"/>
+      <c r="V7" s="101"/>
       <c r="W7" s="44"/>
       <c r="X7" s="44"/>
       <c r="Y7" s="44"/>
@@ -1785,20 +1806,20 @@
       <c r="AR7" s="48"/>
     </row>
     <row r="8" spans="1:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="92"/>
+      <c r="A8" s="103"/>
       <c r="B8" s="44"/>
       <c r="C8" s="68" t="s">
         <v>8</v>
       </c>
       <c r="D8" s="59"/>
-      <c r="E8" s="44"/>
-      <c r="F8" s="69"/>
-      <c r="G8" s="69"/>
-      <c r="H8" s="69"/>
-      <c r="I8" s="69"/>
-      <c r="J8" s="69"/>
-      <c r="K8" s="69"/>
-      <c r="L8" s="69"/>
+      <c r="E8" s="79"/>
+      <c r="F8" s="80"/>
+      <c r="G8" s="80"/>
+      <c r="H8" s="80"/>
+      <c r="I8" s="80"/>
+      <c r="J8" s="80"/>
+      <c r="K8" s="80"/>
+      <c r="L8" s="80"/>
       <c r="M8" s="69"/>
       <c r="N8" s="69"/>
       <c r="O8" s="69"/>
@@ -1833,10 +1854,10 @@
       <c r="AR8" s="66"/>
     </row>
     <row r="9" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="87" t="s">
+      <c r="A9" s="98" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="70" t="s">
+      <c r="B9" s="81" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="10" t="s">
@@ -1887,14 +1908,14 @@
       <c r="AR9" s="21"/>
     </row>
     <row r="10" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="87"/>
-      <c r="B10" s="70"/>
+      <c r="A10" s="98"/>
+      <c r="B10" s="81"/>
       <c r="C10" s="9" t="s">
         <v>8</v>
       </c>
       <c r="D10" s="60"/>
-      <c r="E10" s="94"/>
-      <c r="F10" s="95"/>
+      <c r="E10" s="71"/>
+      <c r="F10" s="72"/>
       <c r="G10" s="12"/>
       <c r="H10" s="38"/>
       <c r="I10" s="33"/>
@@ -1935,8 +1956,8 @@
       <c r="AR10" s="22"/>
     </row>
     <row r="11" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="87"/>
-      <c r="B11" s="70" t="s">
+      <c r="A11" s="98"/>
+      <c r="B11" s="81" t="s">
         <v>49</v>
       </c>
       <c r="C11" s="11" t="s">
@@ -1987,16 +2008,16 @@
       <c r="AR11" s="22"/>
     </row>
     <row r="12" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="87"/>
-      <c r="B12" s="70"/>
+      <c r="A12" s="98"/>
+      <c r="B12" s="81"/>
       <c r="C12" s="8" t="s">
         <v>8</v>
       </c>
       <c r="D12" s="62"/>
       <c r="E12" s="14"/>
       <c r="F12" s="12"/>
-      <c r="G12" s="95"/>
-      <c r="H12" s="96"/>
+      <c r="G12" s="72"/>
+      <c r="H12" s="73"/>
       <c r="I12" s="33"/>
       <c r="J12" s="13"/>
       <c r="K12" s="13"/>
@@ -2035,8 +2056,8 @@
       <c r="AR12" s="22"/>
     </row>
     <row r="13" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="87"/>
-      <c r="B13" s="70" t="s">
+      <c r="A13" s="98"/>
+      <c r="B13" s="81" t="s">
         <v>48</v>
       </c>
       <c r="C13" s="4" t="s">
@@ -2087,8 +2108,8 @@
       <c r="AR13" s="22"/>
     </row>
     <row r="14" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="88"/>
-      <c r="B14" s="71"/>
+      <c r="A14" s="99"/>
+      <c r="B14" s="82"/>
       <c r="C14" s="5" t="s">
         <v>8</v>
       </c>
@@ -2096,8 +2117,8 @@
       <c r="E14" s="18"/>
       <c r="F14" s="19"/>
       <c r="G14" s="19"/>
-      <c r="H14" s="40"/>
-      <c r="I14" s="34"/>
+      <c r="H14" s="74"/>
+      <c r="I14" s="75"/>
       <c r="J14" s="20"/>
       <c r="K14" s="20"/>
       <c r="L14" s="23"/>
@@ -2135,10 +2156,10 @@
       <c r="AR14" s="23"/>
     </row>
     <row r="15" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="86" t="s">
+      <c r="A15" s="97" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="89" t="s">
+      <c r="B15" s="100" t="s">
         <v>9</v>
       </c>
       <c r="C15" s="10" t="s">
@@ -2189,8 +2210,8 @@
       <c r="AR15" s="27"/>
     </row>
     <row r="16" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="87"/>
-      <c r="B16" s="70"/>
+      <c r="A16" s="98"/>
+      <c r="B16" s="81"/>
       <c r="C16" s="8" t="s">
         <v>8</v>
       </c>
@@ -2199,8 +2220,8 @@
       <c r="F16" s="12"/>
       <c r="G16" s="12"/>
       <c r="H16" s="38"/>
-      <c r="I16" s="33"/>
-      <c r="J16" s="13"/>
+      <c r="I16" s="76"/>
+      <c r="J16" s="77"/>
       <c r="K16" s="13"/>
       <c r="L16" s="22"/>
       <c r="M16" s="33"/>
@@ -2237,8 +2258,8 @@
       <c r="AR16" s="22"/>
     </row>
     <row r="17" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="87"/>
-      <c r="B17" s="70" t="s">
+      <c r="A17" s="98"/>
+      <c r="B17" s="81" t="s">
         <v>10</v>
       </c>
       <c r="C17" s="11" t="s">
@@ -2289,8 +2310,8 @@
       <c r="AR17" s="22"/>
     </row>
     <row r="18" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="87"/>
-      <c r="B18" s="70"/>
+      <c r="A18" s="98"/>
+      <c r="B18" s="81"/>
       <c r="C18" s="8" t="s">
         <v>8</v>
       </c>
@@ -2301,8 +2322,8 @@
       <c r="H18" s="38"/>
       <c r="I18" s="33"/>
       <c r="J18" s="13"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="22"/>
+      <c r="K18" s="77"/>
+      <c r="L18" s="78"/>
       <c r="M18" s="33"/>
       <c r="N18" s="13"/>
       <c r="O18" s="13"/>
@@ -2337,8 +2358,8 @@
       <c r="AR18" s="22"/>
     </row>
     <row r="19" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="87"/>
-      <c r="B19" s="70" t="s">
+      <c r="A19" s="98"/>
+      <c r="B19" s="81" t="s">
         <v>16</v>
       </c>
       <c r="C19" s="11" t="s">
@@ -2389,8 +2410,8 @@
       <c r="AR19" s="22"/>
     </row>
     <row r="20" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="87"/>
-      <c r="B20" s="70"/>
+      <c r="A20" s="98"/>
+      <c r="B20" s="81"/>
       <c r="C20" s="8" t="s">
         <v>8</v>
       </c>
@@ -2437,8 +2458,8 @@
       <c r="AR20" s="22"/>
     </row>
     <row r="21" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="87"/>
-      <c r="B21" s="70" t="s">
+      <c r="A21" s="98"/>
+      <c r="B21" s="81" t="s">
         <v>17</v>
       </c>
       <c r="C21" s="11" t="s">
@@ -2489,8 +2510,8 @@
       <c r="AR21" s="22"/>
     </row>
     <row r="22" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="87"/>
-      <c r="B22" s="70"/>
+      <c r="A22" s="98"/>
+      <c r="B22" s="81"/>
       <c r="C22" s="8" t="s">
         <v>8</v>
       </c>
@@ -2537,8 +2558,8 @@
       <c r="AR22" s="22"/>
     </row>
     <row r="23" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="87"/>
-      <c r="B23" s="70" t="s">
+      <c r="A23" s="98"/>
+      <c r="B23" s="81" t="s">
         <v>14</v>
       </c>
       <c r="C23" s="11" t="s">
@@ -2589,8 +2610,8 @@
       <c r="AR23" s="22"/>
     </row>
     <row r="24" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="87"/>
-      <c r="B24" s="70"/>
+      <c r="A24" s="98"/>
+      <c r="B24" s="81"/>
       <c r="C24" s="8" t="s">
         <v>8</v>
       </c>
@@ -2637,8 +2658,8 @@
       <c r="AR24" s="22"/>
     </row>
     <row r="25" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="87"/>
-      <c r="B25" s="70" t="s">
+      <c r="A25" s="98"/>
+      <c r="B25" s="81" t="s">
         <v>15</v>
       </c>
       <c r="C25" s="4" t="s">
@@ -2689,8 +2710,8 @@
       <c r="AR25" s="22"/>
     </row>
     <row r="26" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="88"/>
-      <c r="B26" s="71"/>
+      <c r="A26" s="99"/>
+      <c r="B26" s="82"/>
       <c r="C26" s="5" t="s">
         <v>8</v>
       </c>
@@ -2737,10 +2758,10 @@
       <c r="AR26" s="23"/>
     </row>
     <row r="27" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="87" t="s">
+      <c r="A27" s="98" t="s">
         <v>18</v>
       </c>
-      <c r="B27" s="70" t="s">
+      <c r="B27" s="81" t="s">
         <v>19</v>
       </c>
       <c r="C27" s="7" t="s">
@@ -2791,8 +2812,8 @@
       <c r="AR27" s="27"/>
     </row>
     <row r="28" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="87"/>
-      <c r="B28" s="70"/>
+      <c r="A28" s="98"/>
+      <c r="B28" s="81"/>
       <c r="C28" s="8" t="s">
         <v>8</v>
       </c>
@@ -2839,8 +2860,8 @@
       <c r="AR28" s="22"/>
     </row>
     <row r="29" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="87"/>
-      <c r="B29" s="70" t="s">
+      <c r="A29" s="98"/>
+      <c r="B29" s="81" t="s">
         <v>20</v>
       </c>
       <c r="C29" s="4" t="s">
@@ -2891,8 +2912,8 @@
       <c r="AR29" s="22"/>
     </row>
     <row r="30" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="87"/>
-      <c r="B30" s="70"/>
+      <c r="A30" s="98"/>
+      <c r="B30" s="81"/>
       <c r="C30" s="4" t="s">
         <v>8</v>
       </c>
@@ -2939,7 +2960,7 @@
       <c r="AR30" s="23"/>
     </row>
     <row r="31" spans="1:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="92" t="s">
+      <c r="A31" s="103" t="s">
         <v>11</v>
       </c>
       <c r="B31" s="44"/>
@@ -2968,31 +2989,31 @@
       <c r="T31" s="44"/>
       <c r="U31" s="44"/>
       <c r="V31" s="44"/>
-      <c r="W31" s="90"/>
-      <c r="X31" s="90"/>
-      <c r="Y31" s="90"/>
-      <c r="Z31" s="90"/>
-      <c r="AA31" s="90"/>
-      <c r="AB31" s="90"/>
-      <c r="AC31" s="90"/>
-      <c r="AD31" s="90"/>
-      <c r="AE31" s="90"/>
-      <c r="AF31" s="90"/>
-      <c r="AG31" s="90"/>
-      <c r="AH31" s="90"/>
-      <c r="AI31" s="90"/>
-      <c r="AJ31" s="90"/>
-      <c r="AK31" s="90"/>
-      <c r="AL31" s="90"/>
-      <c r="AM31" s="90"/>
-      <c r="AN31" s="90"/>
-      <c r="AO31" s="90"/>
-      <c r="AP31" s="90"/>
-      <c r="AQ31" s="90"/>
-      <c r="AR31" s="91"/>
+      <c r="W31" s="101"/>
+      <c r="X31" s="101"/>
+      <c r="Y31" s="101"/>
+      <c r="Z31" s="101"/>
+      <c r="AA31" s="101"/>
+      <c r="AB31" s="101"/>
+      <c r="AC31" s="101"/>
+      <c r="AD31" s="101"/>
+      <c r="AE31" s="101"/>
+      <c r="AF31" s="101"/>
+      <c r="AG31" s="101"/>
+      <c r="AH31" s="101"/>
+      <c r="AI31" s="101"/>
+      <c r="AJ31" s="101"/>
+      <c r="AK31" s="101"/>
+      <c r="AL31" s="101"/>
+      <c r="AM31" s="101"/>
+      <c r="AN31" s="101"/>
+      <c r="AO31" s="101"/>
+      <c r="AP31" s="101"/>
+      <c r="AQ31" s="101"/>
+      <c r="AR31" s="102"/>
     </row>
     <row r="32" spans="1:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="92"/>
+      <c r="A32" s="103"/>
       <c r="B32" s="44"/>
       <c r="C32" s="68" t="s">
         <v>8</v>
@@ -3040,10 +3061,10 @@
       <c r="AR32" s="48"/>
     </row>
     <row r="33" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="87" t="s">
+      <c r="A33" s="98" t="s">
         <v>21</v>
       </c>
-      <c r="B33" s="70" t="s">
+      <c r="B33" s="81" t="s">
         <v>51</v>
       </c>
       <c r="C33" s="7" t="s">
@@ -3094,8 +3115,8 @@
       <c r="AR33" s="21"/>
     </row>
     <row r="34" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="87"/>
-      <c r="B34" s="70"/>
+      <c r="A34" s="98"/>
+      <c r="B34" s="81"/>
       <c r="C34" s="8" t="s">
         <v>8</v>
       </c>
@@ -3142,8 +3163,8 @@
       <c r="AR34" s="22"/>
     </row>
     <row r="35" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="87"/>
-      <c r="B35" s="85" t="s">
+      <c r="A35" s="98"/>
+      <c r="B35" s="96" t="s">
         <v>52</v>
       </c>
       <c r="C35" s="11" t="s">
@@ -3194,8 +3215,8 @@
       <c r="AR35" s="22"/>
     </row>
     <row r="36" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="87"/>
-      <c r="B36" s="85"/>
+      <c r="A36" s="98"/>
+      <c r="B36" s="96"/>
       <c r="C36" s="8" t="s">
         <v>8</v>
       </c>
@@ -3242,8 +3263,8 @@
       <c r="AR36" s="22"/>
     </row>
     <row r="37" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="87"/>
-      <c r="B37" s="70" t="s">
+      <c r="A37" s="98"/>
+      <c r="B37" s="81" t="s">
         <v>22</v>
       </c>
       <c r="C37" s="11" t="s">
@@ -3294,8 +3315,8 @@
       <c r="AR37" s="22"/>
     </row>
     <row r="38" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="87"/>
-      <c r="B38" s="70"/>
+      <c r="A38" s="98"/>
+      <c r="B38" s="81"/>
       <c r="C38" s="8" t="s">
         <v>8</v>
       </c>
@@ -3342,8 +3363,8 @@
       <c r="AR38" s="22"/>
     </row>
     <row r="39" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="87"/>
-      <c r="B39" s="70" t="s">
+      <c r="A39" s="98"/>
+      <c r="B39" s="81" t="s">
         <v>23</v>
       </c>
       <c r="C39" s="4" t="s">
@@ -3394,8 +3415,8 @@
       <c r="AR39" s="22"/>
     </row>
     <row r="40" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="88"/>
-      <c r="B40" s="71"/>
+      <c r="A40" s="99"/>
+      <c r="B40" s="82"/>
       <c r="C40" s="5" t="s">
         <v>8</v>
       </c>
@@ -3442,10 +3463,10 @@
       <c r="AR40" s="23"/>
     </row>
     <row r="41" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="86" t="s">
+      <c r="A41" s="97" t="s">
         <v>24</v>
       </c>
-      <c r="B41" s="89" t="s">
+      <c r="B41" s="100" t="s">
         <v>25</v>
       </c>
       <c r="C41" s="10" t="s">
@@ -3496,8 +3517,8 @@
       <c r="AR41" s="27"/>
     </row>
     <row r="42" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="87"/>
-      <c r="B42" s="70"/>
+      <c r="A42" s="98"/>
+      <c r="B42" s="81"/>
       <c r="C42" s="8" t="s">
         <v>8</v>
       </c>
@@ -3544,8 +3565,8 @@
       <c r="AR42" s="22"/>
     </row>
     <row r="43" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="87"/>
-      <c r="B43" s="70" t="s">
+      <c r="A43" s="98"/>
+      <c r="B43" s="81" t="s">
         <v>26</v>
       </c>
       <c r="C43" s="11" t="s">
@@ -3596,8 +3617,8 @@
       <c r="AR43" s="22"/>
     </row>
     <row r="44" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="87"/>
-      <c r="B44" s="70"/>
+      <c r="A44" s="98"/>
+      <c r="B44" s="81"/>
       <c r="C44" s="8" t="s">
         <v>8</v>
       </c>
@@ -3644,8 +3665,8 @@
       <c r="AR44" s="22"/>
     </row>
     <row r="45" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="87"/>
-      <c r="B45" s="70" t="s">
+      <c r="A45" s="98"/>
+      <c r="B45" s="81" t="s">
         <v>53</v>
       </c>
       <c r="C45" s="4" t="s">
@@ -3696,8 +3717,8 @@
       <c r="AR45" s="22"/>
     </row>
     <row r="46" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="88"/>
-      <c r="B46" s="71"/>
+      <c r="A46" s="99"/>
+      <c r="B46" s="82"/>
       <c r="C46" s="5" t="s">
         <v>8</v>
       </c>
@@ -3744,10 +3765,10 @@
       <c r="AR46" s="23"/>
     </row>
     <row r="47" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="86" t="s">
+      <c r="A47" s="97" t="s">
         <v>18</v>
       </c>
-      <c r="B47" s="89" t="s">
+      <c r="B47" s="100" t="s">
         <v>27</v>
       </c>
       <c r="C47" s="10" t="s">
@@ -3798,8 +3819,8 @@
       <c r="AR47" s="27"/>
     </row>
     <row r="48" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="87"/>
-      <c r="B48" s="70"/>
+      <c r="A48" s="98"/>
+      <c r="B48" s="81"/>
       <c r="C48" s="8" t="s">
         <v>8</v>
       </c>
@@ -3846,8 +3867,8 @@
       <c r="AR48" s="22"/>
     </row>
     <row r="49" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="87"/>
-      <c r="B49" s="70" t="s">
+      <c r="A49" s="98"/>
+      <c r="B49" s="81" t="s">
         <v>23</v>
       </c>
       <c r="C49" s="4" t="s">
@@ -3898,8 +3919,8 @@
       <c r="AR49" s="31"/>
     </row>
     <row r="50" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="88"/>
-      <c r="B50" s="71"/>
+      <c r="A50" s="99"/>
+      <c r="B50" s="82"/>
       <c r="C50" s="5" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
Started #14 & #10
Mit Plan-Ansicht begonnen
</commit_message>
<xml_diff>
--- a/docs/ZeitplanIST.xlsx
+++ b/docs/ZeitplanIST.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mail\Code\pelan\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E353820-8084-461B-96BA-AD07C54837F6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A8201EB-4299-4AB0-A6B3-1E10575DA786}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="41235" yWindow="6060" windowWidth="20355" windowHeight="12765" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="54">
   <si>
     <t>Zeitplan</t>
   </si>
@@ -926,73 +926,73 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1321,7 +1321,7 @@
   <dimension ref="A1:AR50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="S16" sqref="S16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1337,198 +1337,198 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:44" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="95" t="s">
+      <c r="A1" s="91" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="95"/>
-      <c r="C1" s="95"/>
-      <c r="D1" s="95"/>
-      <c r="E1" s="95"/>
-      <c r="F1" s="95"/>
-      <c r="G1" s="95"/>
-      <c r="H1" s="95"/>
-      <c r="I1" s="95"/>
-      <c r="J1" s="95"/>
-      <c r="K1" s="95"/>
-      <c r="L1" s="95"/>
-      <c r="M1" s="95"/>
-      <c r="N1" s="95"/>
-      <c r="O1" s="95"/>
-      <c r="P1" s="95"/>
-      <c r="Q1" s="95"/>
-      <c r="R1" s="95"/>
-      <c r="S1" s="95"/>
-      <c r="T1" s="95"/>
-      <c r="U1" s="95"/>
-      <c r="V1" s="95"/>
-      <c r="W1" s="95"/>
-      <c r="X1" s="95"/>
-      <c r="Y1" s="95"/>
-      <c r="Z1" s="95"/>
-      <c r="AA1" s="95"/>
-      <c r="AB1" s="95"/>
-      <c r="AC1" s="95"/>
-      <c r="AD1" s="95"/>
-      <c r="AE1" s="95"/>
-      <c r="AF1" s="95"/>
-      <c r="AG1" s="95"/>
-      <c r="AH1" s="95"/>
-      <c r="AI1" s="95"/>
-      <c r="AJ1" s="95"/>
-      <c r="AK1" s="95"/>
-      <c r="AL1" s="95"/>
-      <c r="AM1" s="95"/>
-      <c r="AN1" s="95"/>
-      <c r="AO1" s="95"/>
-      <c r="AP1" s="95"/>
-      <c r="AQ1" s="95"/>
-      <c r="AR1" s="95"/>
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="91"/>
+      <c r="G1" s="91"/>
+      <c r="H1" s="91"/>
+      <c r="I1" s="91"/>
+      <c r="J1" s="91"/>
+      <c r="K1" s="91"/>
+      <c r="L1" s="91"/>
+      <c r="M1" s="91"/>
+      <c r="N1" s="91"/>
+      <c r="O1" s="91"/>
+      <c r="P1" s="91"/>
+      <c r="Q1" s="91"/>
+      <c r="R1" s="91"/>
+      <c r="S1" s="91"/>
+      <c r="T1" s="91"/>
+      <c r="U1" s="91"/>
+      <c r="V1" s="91"/>
+      <c r="W1" s="91"/>
+      <c r="X1" s="91"/>
+      <c r="Y1" s="91"/>
+      <c r="Z1" s="91"/>
+      <c r="AA1" s="91"/>
+      <c r="AB1" s="91"/>
+      <c r="AC1" s="91"/>
+      <c r="AD1" s="91"/>
+      <c r="AE1" s="91"/>
+      <c r="AF1" s="91"/>
+      <c r="AG1" s="91"/>
+      <c r="AH1" s="91"/>
+      <c r="AI1" s="91"/>
+      <c r="AJ1" s="91"/>
+      <c r="AK1" s="91"/>
+      <c r="AL1" s="91"/>
+      <c r="AM1" s="91"/>
+      <c r="AN1" s="91"/>
+      <c r="AO1" s="91"/>
+      <c r="AP1" s="91"/>
+      <c r="AQ1" s="91"/>
+      <c r="AR1" s="91"/>
     </row>
     <row r="2" spans="1:44" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="92" t="s">
+      <c r="A2" s="100" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="93"/>
-      <c r="C2" s="84" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="86"/>
-      <c r="E2" s="84" t="s">
+      <c r="B2" s="101"/>
+      <c r="C2" s="92" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="94"/>
+      <c r="E2" s="92" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="84" t="s">
+      <c r="F2" s="93"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="94"/>
+      <c r="I2" s="92" t="s">
         <v>38</v>
       </c>
-      <c r="J2" s="85"/>
-      <c r="K2" s="85"/>
-      <c r="L2" s="86"/>
-      <c r="M2" s="84" t="s">
+      <c r="J2" s="93"/>
+      <c r="K2" s="93"/>
+      <c r="L2" s="94"/>
+      <c r="M2" s="92" t="s">
         <v>39</v>
       </c>
-      <c r="N2" s="85"/>
-      <c r="O2" s="85"/>
-      <c r="P2" s="86"/>
-      <c r="Q2" s="84" t="s">
+      <c r="N2" s="93"/>
+      <c r="O2" s="93"/>
+      <c r="P2" s="94"/>
+      <c r="Q2" s="92" t="s">
         <v>40</v>
       </c>
-      <c r="R2" s="85"/>
-      <c r="S2" s="85"/>
-      <c r="T2" s="86"/>
-      <c r="U2" s="84" t="s">
+      <c r="R2" s="93"/>
+      <c r="S2" s="93"/>
+      <c r="T2" s="94"/>
+      <c r="U2" s="92" t="s">
         <v>41</v>
       </c>
-      <c r="V2" s="85"/>
-      <c r="W2" s="85"/>
-      <c r="X2" s="86"/>
-      <c r="Y2" s="84" t="s">
+      <c r="V2" s="93"/>
+      <c r="W2" s="93"/>
+      <c r="X2" s="94"/>
+      <c r="Y2" s="92" t="s">
         <v>42</v>
       </c>
-      <c r="Z2" s="85"/>
-      <c r="AA2" s="85"/>
-      <c r="AB2" s="86"/>
-      <c r="AC2" s="84" t="s">
+      <c r="Z2" s="93"/>
+      <c r="AA2" s="93"/>
+      <c r="AB2" s="94"/>
+      <c r="AC2" s="92" t="s">
         <v>43</v>
       </c>
-      <c r="AD2" s="85"/>
-      <c r="AE2" s="85"/>
-      <c r="AF2" s="86"/>
-      <c r="AG2" s="84" t="s">
+      <c r="AD2" s="93"/>
+      <c r="AE2" s="93"/>
+      <c r="AF2" s="94"/>
+      <c r="AG2" s="92" t="s">
         <v>44</v>
       </c>
-      <c r="AH2" s="85"/>
-      <c r="AI2" s="85"/>
-      <c r="AJ2" s="86"/>
-      <c r="AK2" s="84" t="s">
+      <c r="AH2" s="93"/>
+      <c r="AI2" s="93"/>
+      <c r="AJ2" s="94"/>
+      <c r="AK2" s="92" t="s">
         <v>45</v>
       </c>
-      <c r="AL2" s="85"/>
-      <c r="AM2" s="85"/>
-      <c r="AN2" s="86"/>
-      <c r="AO2" s="84" t="s">
+      <c r="AL2" s="93"/>
+      <c r="AM2" s="93"/>
+      <c r="AN2" s="94"/>
+      <c r="AO2" s="92" t="s">
         <v>46</v>
       </c>
-      <c r="AP2" s="85"/>
-      <c r="AQ2" s="85"/>
-      <c r="AR2" s="86"/>
+      <c r="AP2" s="93"/>
+      <c r="AQ2" s="93"/>
+      <c r="AR2" s="94"/>
     </row>
     <row r="3" spans="1:44" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="92"/>
-      <c r="B3" s="93"/>
-      <c r="C3" s="87"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="87" t="s">
+      <c r="A3" s="100"/>
+      <c r="B3" s="101"/>
+      <c r="C3" s="95"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="95" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="88"/>
-      <c r="G3" s="88"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="87" t="s">
+      <c r="F3" s="96"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="95" t="s">
         <v>29</v>
       </c>
-      <c r="J3" s="88"/>
-      <c r="K3" s="88"/>
-      <c r="L3" s="89"/>
-      <c r="M3" s="87" t="s">
+      <c r="J3" s="96"/>
+      <c r="K3" s="96"/>
+      <c r="L3" s="97"/>
+      <c r="M3" s="95" t="s">
         <v>30</v>
       </c>
-      <c r="N3" s="88"/>
-      <c r="O3" s="88"/>
-      <c r="P3" s="89"/>
-      <c r="Q3" s="87" t="s">
+      <c r="N3" s="96"/>
+      <c r="O3" s="96"/>
+      <c r="P3" s="97"/>
+      <c r="Q3" s="95" t="s">
         <v>31</v>
       </c>
-      <c r="R3" s="88"/>
-      <c r="S3" s="88"/>
-      <c r="T3" s="89"/>
-      <c r="U3" s="87" t="s">
+      <c r="R3" s="96"/>
+      <c r="S3" s="96"/>
+      <c r="T3" s="97"/>
+      <c r="U3" s="95" t="s">
         <v>32</v>
       </c>
-      <c r="V3" s="88"/>
-      <c r="W3" s="88"/>
-      <c r="X3" s="89"/>
-      <c r="Y3" s="87" t="s">
+      <c r="V3" s="96"/>
+      <c r="W3" s="96"/>
+      <c r="X3" s="97"/>
+      <c r="Y3" s="95" t="s">
         <v>33</v>
       </c>
-      <c r="Z3" s="88"/>
-      <c r="AA3" s="88"/>
-      <c r="AB3" s="89"/>
-      <c r="AC3" s="87" t="s">
+      <c r="Z3" s="96"/>
+      <c r="AA3" s="96"/>
+      <c r="AB3" s="97"/>
+      <c r="AC3" s="95" t="s">
         <v>34</v>
       </c>
-      <c r="AD3" s="88"/>
-      <c r="AE3" s="88"/>
-      <c r="AF3" s="89"/>
-      <c r="AG3" s="87" t="s">
+      <c r="AD3" s="96"/>
+      <c r="AE3" s="96"/>
+      <c r="AF3" s="97"/>
+      <c r="AG3" s="95" t="s">
         <v>35</v>
       </c>
-      <c r="AH3" s="88"/>
-      <c r="AI3" s="88"/>
-      <c r="AJ3" s="89"/>
-      <c r="AK3" s="87" t="s">
+      <c r="AH3" s="96"/>
+      <c r="AI3" s="96"/>
+      <c r="AJ3" s="97"/>
+      <c r="AK3" s="95" t="s">
         <v>36</v>
       </c>
-      <c r="AL3" s="88"/>
-      <c r="AM3" s="88"/>
-      <c r="AN3" s="89"/>
-      <c r="AO3" s="87" t="s">
+      <c r="AL3" s="96"/>
+      <c r="AM3" s="96"/>
+      <c r="AN3" s="97"/>
+      <c r="AO3" s="95" t="s">
         <v>37</v>
       </c>
-      <c r="AP3" s="88"/>
-      <c r="AQ3" s="88"/>
-      <c r="AR3" s="89"/>
+      <c r="AP3" s="96"/>
+      <c r="AQ3" s="96"/>
+      <c r="AR3" s="97"/>
     </row>
     <row r="4" spans="1:44" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="90" t="s">
+      <c r="A4" s="98" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="91"/>
-      <c r="C4" s="94" t="s">
+      <c r="B4" s="99"/>
+      <c r="C4" s="102" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="91"/>
+      <c r="D4" s="99"/>
       <c r="E4" s="45">
         <v>2</v>
       </c>
@@ -1651,10 +1651,10 @@
       </c>
     </row>
     <row r="5" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="83" t="s">
+      <c r="A5" s="103" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="81" t="s">
+      <c r="B5" s="83" t="s">
         <v>50</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -1705,8 +1705,8 @@
       <c r="AR5" s="22"/>
     </row>
     <row r="6" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="84"/>
-      <c r="B6" s="81"/>
+      <c r="A6" s="92"/>
+      <c r="B6" s="83"/>
       <c r="C6" s="4" t="s">
         <v>8</v>
       </c>
@@ -1753,7 +1753,7 @@
       <c r="AR6" s="23"/>
     </row>
     <row r="7" spans="1:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="103" t="s">
+      <c r="A7" s="89" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="44"/>
@@ -1765,23 +1765,23 @@
         <v>34</v>
       </c>
       <c r="E7" s="44"/>
-      <c r="F7" s="101"/>
-      <c r="G7" s="101"/>
-      <c r="H7" s="101"/>
-      <c r="I7" s="101"/>
-      <c r="J7" s="101"/>
-      <c r="K7" s="101"/>
-      <c r="L7" s="101"/>
-      <c r="M7" s="101"/>
-      <c r="N7" s="101"/>
-      <c r="O7" s="101"/>
-      <c r="P7" s="101"/>
-      <c r="Q7" s="101"/>
-      <c r="R7" s="101"/>
-      <c r="S7" s="101"/>
-      <c r="T7" s="101"/>
-      <c r="U7" s="101"/>
-      <c r="V7" s="101"/>
+      <c r="F7" s="81"/>
+      <c r="G7" s="81"/>
+      <c r="H7" s="81"/>
+      <c r="I7" s="81"/>
+      <c r="J7" s="81"/>
+      <c r="K7" s="81"/>
+      <c r="L7" s="81"/>
+      <c r="M7" s="81"/>
+      <c r="N7" s="81"/>
+      <c r="O7" s="81"/>
+      <c r="P7" s="81"/>
+      <c r="Q7" s="81"/>
+      <c r="R7" s="81"/>
+      <c r="S7" s="81"/>
+      <c r="T7" s="81"/>
+      <c r="U7" s="81"/>
+      <c r="V7" s="81"/>
       <c r="W7" s="44"/>
       <c r="X7" s="44"/>
       <c r="Y7" s="44"/>
@@ -1806,7 +1806,7 @@
       <c r="AR7" s="48"/>
     </row>
     <row r="8" spans="1:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="103"/>
+      <c r="A8" s="89"/>
       <c r="B8" s="44"/>
       <c r="C8" s="68" t="s">
         <v>8</v>
@@ -1820,10 +1820,10 @@
       <c r="J8" s="80"/>
       <c r="K8" s="80"/>
       <c r="L8" s="80"/>
-      <c r="M8" s="69"/>
-      <c r="N8" s="69"/>
-      <c r="O8" s="69"/>
-      <c r="P8" s="69"/>
+      <c r="M8" s="80"/>
+      <c r="N8" s="80"/>
+      <c r="O8" s="80"/>
+      <c r="P8" s="80"/>
       <c r="Q8" s="69"/>
       <c r="R8" s="69"/>
       <c r="S8" s="69"/>
@@ -1854,10 +1854,10 @@
       <c r="AR8" s="66"/>
     </row>
     <row r="9" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="98" t="s">
+      <c r="A9" s="84" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="81" t="s">
+      <c r="B9" s="83" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="10" t="s">
@@ -1908,8 +1908,8 @@
       <c r="AR9" s="21"/>
     </row>
     <row r="10" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="98"/>
-      <c r="B10" s="81"/>
+      <c r="A10" s="84"/>
+      <c r="B10" s="83"/>
       <c r="C10" s="9" t="s">
         <v>8</v>
       </c>
@@ -1956,8 +1956,8 @@
       <c r="AR10" s="22"/>
     </row>
     <row r="11" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="98"/>
-      <c r="B11" s="81" t="s">
+      <c r="A11" s="84"/>
+      <c r="B11" s="83" t="s">
         <v>49</v>
       </c>
       <c r="C11" s="11" t="s">
@@ -2008,8 +2008,8 @@
       <c r="AR11" s="22"/>
     </row>
     <row r="12" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="98"/>
-      <c r="B12" s="81"/>
+      <c r="A12" s="84"/>
+      <c r="B12" s="83"/>
       <c r="C12" s="8" t="s">
         <v>8</v>
       </c>
@@ -2056,8 +2056,8 @@
       <c r="AR12" s="22"/>
     </row>
     <row r="13" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="98"/>
-      <c r="B13" s="81" t="s">
+      <c r="A13" s="84"/>
+      <c r="B13" s="83" t="s">
         <v>48</v>
       </c>
       <c r="C13" s="4" t="s">
@@ -2108,8 +2108,8 @@
       <c r="AR13" s="22"/>
     </row>
     <row r="14" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="99"/>
-      <c r="B14" s="82"/>
+      <c r="A14" s="86"/>
+      <c r="B14" s="87"/>
       <c r="C14" s="5" t="s">
         <v>8</v>
       </c>
@@ -2156,10 +2156,10 @@
       <c r="AR14" s="23"/>
     </row>
     <row r="15" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="97" t="s">
+      <c r="A15" s="88" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="100" t="s">
+      <c r="B15" s="85" t="s">
         <v>9</v>
       </c>
       <c r="C15" s="10" t="s">
@@ -2210,8 +2210,8 @@
       <c r="AR15" s="27"/>
     </row>
     <row r="16" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="98"/>
-      <c r="B16" s="81"/>
+      <c r="A16" s="84"/>
+      <c r="B16" s="83"/>
       <c r="C16" s="8" t="s">
         <v>8</v>
       </c>
@@ -2258,8 +2258,8 @@
       <c r="AR16" s="22"/>
     </row>
     <row r="17" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="98"/>
-      <c r="B17" s="81" t="s">
+      <c r="A17" s="84"/>
+      <c r="B17" s="83" t="s">
         <v>10</v>
       </c>
       <c r="C17" s="11" t="s">
@@ -2310,8 +2310,8 @@
       <c r="AR17" s="22"/>
     </row>
     <row r="18" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="98"/>
-      <c r="B18" s="81"/>
+      <c r="A18" s="84"/>
+      <c r="B18" s="83"/>
       <c r="C18" s="8" t="s">
         <v>8</v>
       </c>
@@ -2358,8 +2358,8 @@
       <c r="AR18" s="22"/>
     </row>
     <row r="19" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="98"/>
-      <c r="B19" s="81" t="s">
+      <c r="A19" s="84"/>
+      <c r="B19" s="83" t="s">
         <v>16</v>
       </c>
       <c r="C19" s="11" t="s">
@@ -2410,8 +2410,8 @@
       <c r="AR19" s="22"/>
     </row>
     <row r="20" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="98"/>
-      <c r="B20" s="81"/>
+      <c r="A20" s="84"/>
+      <c r="B20" s="83"/>
       <c r="C20" s="8" t="s">
         <v>8</v>
       </c>
@@ -2424,10 +2424,10 @@
       <c r="J20" s="13"/>
       <c r="K20" s="13"/>
       <c r="L20" s="22"/>
-      <c r="M20" s="33"/>
-      <c r="N20" s="13"/>
-      <c r="O20" s="13"/>
-      <c r="P20" s="22"/>
+      <c r="M20" s="76"/>
+      <c r="N20" s="77"/>
+      <c r="O20" s="77"/>
+      <c r="P20" s="78"/>
       <c r="Q20" s="33"/>
       <c r="R20" s="13"/>
       <c r="S20" s="13"/>
@@ -2458,8 +2458,8 @@
       <c r="AR20" s="22"/>
     </row>
     <row r="21" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="98"/>
-      <c r="B21" s="81" t="s">
+      <c r="A21" s="84"/>
+      <c r="B21" s="83" t="s">
         <v>17</v>
       </c>
       <c r="C21" s="11" t="s">
@@ -2510,8 +2510,8 @@
       <c r="AR21" s="22"/>
     </row>
     <row r="22" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="98"/>
-      <c r="B22" s="81"/>
+      <c r="A22" s="84"/>
+      <c r="B22" s="83"/>
       <c r="C22" s="8" t="s">
         <v>8</v>
       </c>
@@ -2558,8 +2558,8 @@
       <c r="AR22" s="22"/>
     </row>
     <row r="23" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="98"/>
-      <c r="B23" s="81" t="s">
+      <c r="A23" s="84"/>
+      <c r="B23" s="83" t="s">
         <v>14</v>
       </c>
       <c r="C23" s="11" t="s">
@@ -2610,8 +2610,8 @@
       <c r="AR23" s="22"/>
     </row>
     <row r="24" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="98"/>
-      <c r="B24" s="81"/>
+      <c r="A24" s="84"/>
+      <c r="B24" s="83"/>
       <c r="C24" s="8" t="s">
         <v>8</v>
       </c>
@@ -2658,8 +2658,8 @@
       <c r="AR24" s="22"/>
     </row>
     <row r="25" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="98"/>
-      <c r="B25" s="81" t="s">
+      <c r="A25" s="84"/>
+      <c r="B25" s="83" t="s">
         <v>15</v>
       </c>
       <c r="C25" s="4" t="s">
@@ -2710,8 +2710,8 @@
       <c r="AR25" s="22"/>
     </row>
     <row r="26" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="99"/>
-      <c r="B26" s="82"/>
+      <c r="A26" s="86"/>
+      <c r="B26" s="87"/>
       <c r="C26" s="5" t="s">
         <v>8</v>
       </c>
@@ -2758,10 +2758,10 @@
       <c r="AR26" s="23"/>
     </row>
     <row r="27" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="98" t="s">
+      <c r="A27" s="84" t="s">
         <v>18</v>
       </c>
-      <c r="B27" s="81" t="s">
+      <c r="B27" s="83" t="s">
         <v>19</v>
       </c>
       <c r="C27" s="7" t="s">
@@ -2812,8 +2812,8 @@
       <c r="AR27" s="27"/>
     </row>
     <row r="28" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="98"/>
-      <c r="B28" s="81"/>
+      <c r="A28" s="84"/>
+      <c r="B28" s="83"/>
       <c r="C28" s="8" t="s">
         <v>8</v>
       </c>
@@ -2860,8 +2860,8 @@
       <c r="AR28" s="22"/>
     </row>
     <row r="29" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="98"/>
-      <c r="B29" s="81" t="s">
+      <c r="A29" s="84"/>
+      <c r="B29" s="83" t="s">
         <v>20</v>
       </c>
       <c r="C29" s="4" t="s">
@@ -2912,8 +2912,8 @@
       <c r="AR29" s="22"/>
     </row>
     <row r="30" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="98"/>
-      <c r="B30" s="81"/>
+      <c r="A30" s="84"/>
+      <c r="B30" s="83"/>
       <c r="C30" s="4" t="s">
         <v>8</v>
       </c>
@@ -2960,7 +2960,7 @@
       <c r="AR30" s="23"/>
     </row>
     <row r="31" spans="1:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="103" t="s">
+      <c r="A31" s="89" t="s">
         <v>11</v>
       </c>
       <c r="B31" s="44"/>
@@ -2989,31 +2989,31 @@
       <c r="T31" s="44"/>
       <c r="U31" s="44"/>
       <c r="V31" s="44"/>
-      <c r="W31" s="101"/>
-      <c r="X31" s="101"/>
-      <c r="Y31" s="101"/>
-      <c r="Z31" s="101"/>
-      <c r="AA31" s="101"/>
-      <c r="AB31" s="101"/>
-      <c r="AC31" s="101"/>
-      <c r="AD31" s="101"/>
-      <c r="AE31" s="101"/>
-      <c r="AF31" s="101"/>
-      <c r="AG31" s="101"/>
-      <c r="AH31" s="101"/>
-      <c r="AI31" s="101"/>
-      <c r="AJ31" s="101"/>
-      <c r="AK31" s="101"/>
-      <c r="AL31" s="101"/>
-      <c r="AM31" s="101"/>
-      <c r="AN31" s="101"/>
-      <c r="AO31" s="101"/>
-      <c r="AP31" s="101"/>
-      <c r="AQ31" s="101"/>
-      <c r="AR31" s="102"/>
+      <c r="W31" s="81"/>
+      <c r="X31" s="81"/>
+      <c r="Y31" s="81"/>
+      <c r="Z31" s="81"/>
+      <c r="AA31" s="81"/>
+      <c r="AB31" s="81"/>
+      <c r="AC31" s="81"/>
+      <c r="AD31" s="81"/>
+      <c r="AE31" s="81"/>
+      <c r="AF31" s="81"/>
+      <c r="AG31" s="81"/>
+      <c r="AH31" s="81"/>
+      <c r="AI31" s="81"/>
+      <c r="AJ31" s="81"/>
+      <c r="AK31" s="81"/>
+      <c r="AL31" s="81"/>
+      <c r="AM31" s="81"/>
+      <c r="AN31" s="81"/>
+      <c r="AO31" s="81"/>
+      <c r="AP31" s="81"/>
+      <c r="AQ31" s="81"/>
+      <c r="AR31" s="82"/>
     </row>
     <row r="32" spans="1:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="103"/>
+      <c r="A32" s="89"/>
       <c r="B32" s="44"/>
       <c r="C32" s="68" t="s">
         <v>8</v>
@@ -3061,10 +3061,10 @@
       <c r="AR32" s="48"/>
     </row>
     <row r="33" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="98" t="s">
+      <c r="A33" s="84" t="s">
         <v>21</v>
       </c>
-      <c r="B33" s="81" t="s">
+      <c r="B33" s="83" t="s">
         <v>51</v>
       </c>
       <c r="C33" s="7" t="s">
@@ -3115,8 +3115,8 @@
       <c r="AR33" s="21"/>
     </row>
     <row r="34" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="98"/>
-      <c r="B34" s="81"/>
+      <c r="A34" s="84"/>
+      <c r="B34" s="83"/>
       <c r="C34" s="8" t="s">
         <v>8</v>
       </c>
@@ -3163,8 +3163,8 @@
       <c r="AR34" s="22"/>
     </row>
     <row r="35" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="98"/>
-      <c r="B35" s="96" t="s">
+      <c r="A35" s="84"/>
+      <c r="B35" s="90" t="s">
         <v>52</v>
       </c>
       <c r="C35" s="11" t="s">
@@ -3215,8 +3215,8 @@
       <c r="AR35" s="22"/>
     </row>
     <row r="36" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="98"/>
-      <c r="B36" s="96"/>
+      <c r="A36" s="84"/>
+      <c r="B36" s="90"/>
       <c r="C36" s="8" t="s">
         <v>8</v>
       </c>
@@ -3263,8 +3263,8 @@
       <c r="AR36" s="22"/>
     </row>
     <row r="37" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="98"/>
-      <c r="B37" s="81" t="s">
+      <c r="A37" s="84"/>
+      <c r="B37" s="83" t="s">
         <v>22</v>
       </c>
       <c r="C37" s="11" t="s">
@@ -3315,8 +3315,8 @@
       <c r="AR37" s="22"/>
     </row>
     <row r="38" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="98"/>
-      <c r="B38" s="81"/>
+      <c r="A38" s="84"/>
+      <c r="B38" s="83"/>
       <c r="C38" s="8" t="s">
         <v>8</v>
       </c>
@@ -3363,8 +3363,8 @@
       <c r="AR38" s="22"/>
     </row>
     <row r="39" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="98"/>
-      <c r="B39" s="81" t="s">
+      <c r="A39" s="84"/>
+      <c r="B39" s="83" t="s">
         <v>23</v>
       </c>
       <c r="C39" s="4" t="s">
@@ -3415,8 +3415,8 @@
       <c r="AR39" s="22"/>
     </row>
     <row r="40" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="99"/>
-      <c r="B40" s="82"/>
+      <c r="A40" s="86"/>
+      <c r="B40" s="87"/>
       <c r="C40" s="5" t="s">
         <v>8</v>
       </c>
@@ -3463,10 +3463,10 @@
       <c r="AR40" s="23"/>
     </row>
     <row r="41" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="97" t="s">
+      <c r="A41" s="88" t="s">
         <v>24</v>
       </c>
-      <c r="B41" s="100" t="s">
+      <c r="B41" s="85" t="s">
         <v>25</v>
       </c>
       <c r="C41" s="10" t="s">
@@ -3517,8 +3517,8 @@
       <c r="AR41" s="27"/>
     </row>
     <row r="42" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="98"/>
-      <c r="B42" s="81"/>
+      <c r="A42" s="84"/>
+      <c r="B42" s="83"/>
       <c r="C42" s="8" t="s">
         <v>8</v>
       </c>
@@ -3565,8 +3565,8 @@
       <c r="AR42" s="22"/>
     </row>
     <row r="43" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="98"/>
-      <c r="B43" s="81" t="s">
+      <c r="A43" s="84"/>
+      <c r="B43" s="83" t="s">
         <v>26</v>
       </c>
       <c r="C43" s="11" t="s">
@@ -3617,8 +3617,8 @@
       <c r="AR43" s="22"/>
     </row>
     <row r="44" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="98"/>
-      <c r="B44" s="81"/>
+      <c r="A44" s="84"/>
+      <c r="B44" s="83"/>
       <c r="C44" s="8" t="s">
         <v>8</v>
       </c>
@@ -3665,8 +3665,8 @@
       <c r="AR44" s="22"/>
     </row>
     <row r="45" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="98"/>
-      <c r="B45" s="81" t="s">
+      <c r="A45" s="84"/>
+      <c r="B45" s="83" t="s">
         <v>53</v>
       </c>
       <c r="C45" s="4" t="s">
@@ -3717,8 +3717,8 @@
       <c r="AR45" s="22"/>
     </row>
     <row r="46" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="99"/>
-      <c r="B46" s="82"/>
+      <c r="A46" s="86"/>
+      <c r="B46" s="87"/>
       <c r="C46" s="5" t="s">
         <v>8</v>
       </c>
@@ -3765,10 +3765,10 @@
       <c r="AR46" s="23"/>
     </row>
     <row r="47" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="97" t="s">
+      <c r="A47" s="88" t="s">
         <v>18</v>
       </c>
-      <c r="B47" s="100" t="s">
+      <c r="B47" s="85" t="s">
         <v>27</v>
       </c>
       <c r="C47" s="10" t="s">
@@ -3819,8 +3819,8 @@
       <c r="AR47" s="27"/>
     </row>
     <row r="48" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="98"/>
-      <c r="B48" s="81"/>
+      <c r="A48" s="84"/>
+      <c r="B48" s="83"/>
       <c r="C48" s="8" t="s">
         <v>8</v>
       </c>
@@ -3867,8 +3867,8 @@
       <c r="AR48" s="22"/>
     </row>
     <row r="49" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="98"/>
-      <c r="B49" s="81" t="s">
+      <c r="A49" s="84"/>
+      <c r="B49" s="83" t="s">
         <v>23</v>
       </c>
       <c r="C49" s="4" t="s">
@@ -3919,8 +3919,8 @@
       <c r="AR49" s="31"/>
     </row>
     <row r="50" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="99"/>
-      <c r="B50" s="82"/>
+      <c r="A50" s="86"/>
+      <c r="B50" s="87"/>
       <c r="C50" s="5" t="s">
         <v>8</v>
       </c>
@@ -3968,6 +3968,47 @@
     </row>
   </sheetData>
   <mergeCells count="57">
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="Q2:T2"/>
+    <mergeCell ref="Q3:T3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A2:B3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="C2:D3"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="I3:L3"/>
+    <mergeCell ref="A1:AR1"/>
+    <mergeCell ref="AO2:AR2"/>
+    <mergeCell ref="Y3:AB3"/>
+    <mergeCell ref="AC3:AF3"/>
+    <mergeCell ref="AG3:AJ3"/>
+    <mergeCell ref="AK3:AN3"/>
+    <mergeCell ref="AO3:AR3"/>
+    <mergeCell ref="U2:X2"/>
+    <mergeCell ref="U3:X3"/>
+    <mergeCell ref="Y2:AB2"/>
+    <mergeCell ref="AC2:AF2"/>
+    <mergeCell ref="AG2:AJ2"/>
+    <mergeCell ref="AK2:AN2"/>
+    <mergeCell ref="I2:L2"/>
+    <mergeCell ref="M2:P2"/>
+    <mergeCell ref="M3:P3"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="A47:A50"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="A41:A46"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="A33:A40"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B37:B38"/>
     <mergeCell ref="F7:V7"/>
     <mergeCell ref="W31:AR31"/>
     <mergeCell ref="B29:B30"/>
@@ -3984,47 +4025,6 @@
     <mergeCell ref="B23:B24"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="A31:A32"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="A47:A50"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="A41:A46"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="A33:A40"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="A1:AR1"/>
-    <mergeCell ref="AO2:AR2"/>
-    <mergeCell ref="Y3:AB3"/>
-    <mergeCell ref="AC3:AF3"/>
-    <mergeCell ref="AG3:AJ3"/>
-    <mergeCell ref="AK3:AN3"/>
-    <mergeCell ref="AO3:AR3"/>
-    <mergeCell ref="U2:X2"/>
-    <mergeCell ref="U3:X3"/>
-    <mergeCell ref="Y2:AB2"/>
-    <mergeCell ref="AC2:AF2"/>
-    <mergeCell ref="AG2:AJ2"/>
-    <mergeCell ref="AK2:AN2"/>
-    <mergeCell ref="I2:L2"/>
-    <mergeCell ref="M2:P2"/>
-    <mergeCell ref="M3:P3"/>
-    <mergeCell ref="Q2:T2"/>
-    <mergeCell ref="Q3:T3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A2:B3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E2:H2"/>
-    <mergeCell ref="C2:D3"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="I3:L3"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="53" orientation="landscape" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
Plan done, improoved reactivity, dashboard started
 closes #11, closes #15, closes #20, closes #8, closes #14

- Dienstplan fertig
- Store / Reaktivität gewisser Komponenten verbessert
- Zahlreiche kleinere Verbesserungen / Formatierungen / Kommentare
- Dashboard begonnen
</commit_message>
<xml_diff>
--- a/docs/ZeitplanIST.xlsx
+++ b/docs/ZeitplanIST.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mail\Code\pelan\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE084636-39E5-4D92-A1DB-A4853C004A0C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DD0C2F1-77C0-484A-AC25-255A4583DF79}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="41235" yWindow="6060" windowWidth="20355" windowHeight="12765" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1004,6 +1004,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -1026,15 +1035,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1362,8 +1362,8 @@
   </sheetPr>
   <dimension ref="B2:AS51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="R21" sqref="R21"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1380,52 +1380,52 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:45" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B2" s="103" t="s">
+      <c r="B2" s="95" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="104"/>
-      <c r="D2" s="104"/>
-      <c r="E2" s="104"/>
-      <c r="F2" s="104"/>
-      <c r="G2" s="104"/>
-      <c r="H2" s="104"/>
-      <c r="I2" s="104"/>
-      <c r="J2" s="104"/>
-      <c r="K2" s="104"/>
-      <c r="L2" s="104"/>
-      <c r="M2" s="104"/>
-      <c r="N2" s="104"/>
-      <c r="O2" s="104"/>
-      <c r="P2" s="104"/>
-      <c r="Q2" s="104"/>
-      <c r="R2" s="104"/>
-      <c r="S2" s="104"/>
-      <c r="T2" s="104"/>
-      <c r="U2" s="104"/>
-      <c r="V2" s="104"/>
-      <c r="W2" s="104"/>
-      <c r="X2" s="104"/>
-      <c r="Y2" s="104"/>
-      <c r="Z2" s="104"/>
-      <c r="AA2" s="104"/>
-      <c r="AB2" s="104"/>
-      <c r="AC2" s="104"/>
-      <c r="AD2" s="104"/>
-      <c r="AE2" s="104"/>
-      <c r="AF2" s="104"/>
-      <c r="AG2" s="104"/>
-      <c r="AH2" s="104"/>
-      <c r="AI2" s="104"/>
-      <c r="AJ2" s="104"/>
-      <c r="AK2" s="104"/>
-      <c r="AL2" s="104"/>
-      <c r="AM2" s="104"/>
-      <c r="AN2" s="104"/>
-      <c r="AO2" s="104"/>
-      <c r="AP2" s="104"/>
-      <c r="AQ2" s="104"/>
-      <c r="AR2" s="104"/>
-      <c r="AS2" s="105"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="96"/>
+      <c r="I2" s="96"/>
+      <c r="J2" s="96"/>
+      <c r="K2" s="96"/>
+      <c r="L2" s="96"/>
+      <c r="M2" s="96"/>
+      <c r="N2" s="96"/>
+      <c r="O2" s="96"/>
+      <c r="P2" s="96"/>
+      <c r="Q2" s="96"/>
+      <c r="R2" s="96"/>
+      <c r="S2" s="96"/>
+      <c r="T2" s="96"/>
+      <c r="U2" s="96"/>
+      <c r="V2" s="96"/>
+      <c r="W2" s="96"/>
+      <c r="X2" s="96"/>
+      <c r="Y2" s="96"/>
+      <c r="Z2" s="96"/>
+      <c r="AA2" s="96"/>
+      <c r="AB2" s="96"/>
+      <c r="AC2" s="96"/>
+      <c r="AD2" s="96"/>
+      <c r="AE2" s="96"/>
+      <c r="AF2" s="96"/>
+      <c r="AG2" s="96"/>
+      <c r="AH2" s="96"/>
+      <c r="AI2" s="96"/>
+      <c r="AJ2" s="96"/>
+      <c r="AK2" s="96"/>
+      <c r="AL2" s="96"/>
+      <c r="AM2" s="96"/>
+      <c r="AN2" s="96"/>
+      <c r="AO2" s="96"/>
+      <c r="AP2" s="96"/>
+      <c r="AQ2" s="96"/>
+      <c r="AR2" s="96"/>
+      <c r="AS2" s="97"/>
     </row>
     <row r="3" spans="2:45" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="92" t="s">
@@ -1798,7 +1798,7 @@
       <c r="AS7" s="23"/>
     </row>
     <row r="8" spans="2:45" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="102" t="s">
+      <c r="B8" s="105" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="44"/>
@@ -1810,23 +1810,23 @@
         <v>34</v>
       </c>
       <c r="F8" s="44"/>
-      <c r="G8" s="100"/>
-      <c r="H8" s="100"/>
-      <c r="I8" s="100"/>
-      <c r="J8" s="100"/>
-      <c r="K8" s="100"/>
-      <c r="L8" s="100"/>
-      <c r="M8" s="100"/>
-      <c r="N8" s="100"/>
-      <c r="O8" s="100"/>
-      <c r="P8" s="100"/>
-      <c r="Q8" s="100"/>
-      <c r="R8" s="100"/>
-      <c r="S8" s="100"/>
-      <c r="T8" s="100"/>
-      <c r="U8" s="100"/>
-      <c r="V8" s="100"/>
-      <c r="W8" s="100"/>
+      <c r="G8" s="103"/>
+      <c r="H8" s="103"/>
+      <c r="I8" s="103"/>
+      <c r="J8" s="103"/>
+      <c r="K8" s="103"/>
+      <c r="L8" s="103"/>
+      <c r="M8" s="103"/>
+      <c r="N8" s="103"/>
+      <c r="O8" s="103"/>
+      <c r="P8" s="103"/>
+      <c r="Q8" s="103"/>
+      <c r="R8" s="103"/>
+      <c r="S8" s="103"/>
+      <c r="T8" s="103"/>
+      <c r="U8" s="103"/>
+      <c r="V8" s="103"/>
+      <c r="W8" s="103"/>
       <c r="X8" s="44"/>
       <c r="Y8" s="44"/>
       <c r="Z8" s="44"/>
@@ -1851,14 +1851,14 @@
       <c r="AS8" s="48"/>
     </row>
     <row r="9" spans="2:45" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="102"/>
+      <c r="B9" s="105"/>
       <c r="C9" s="44"/>
       <c r="D9" s="68" t="s">
         <v>8</v>
       </c>
       <c r="E9" s="67">
         <f>SUM(E11+E13+E15+E17+E19+E21+E23+E25+E27+E29+E31)</f>
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="F9" s="79"/>
       <c r="G9" s="80"/>
@@ -1873,9 +1873,9 @@
       <c r="P9" s="80"/>
       <c r="Q9" s="80"/>
       <c r="R9" s="80"/>
-      <c r="S9" s="69"/>
-      <c r="T9" s="69"/>
-      <c r="U9" s="69"/>
+      <c r="S9" s="80"/>
+      <c r="T9" s="80"/>
+      <c r="U9" s="80"/>
       <c r="V9" s="69"/>
       <c r="W9" s="69"/>
       <c r="X9" s="44"/>
@@ -1902,7 +1902,7 @@
       <c r="AS9" s="66"/>
     </row>
     <row r="10" spans="2:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="97" t="s">
+      <c r="B10" s="100" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="81" t="s">
@@ -1956,7 +1956,7 @@
       <c r="AS10" s="21"/>
     </row>
     <row r="11" spans="2:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="97"/>
+      <c r="B11" s="100"/>
       <c r="C11" s="81"/>
       <c r="D11" s="9" t="s">
         <v>8</v>
@@ -2006,7 +2006,7 @@
       <c r="AS11" s="22"/>
     </row>
     <row r="12" spans="2:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="97"/>
+      <c r="B12" s="100"/>
       <c r="C12" s="81" t="s">
         <v>47</v>
       </c>
@@ -2058,7 +2058,7 @@
       <c r="AS12" s="22"/>
     </row>
     <row r="13" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="97"/>
+      <c r="B13" s="100"/>
       <c r="C13" s="81"/>
       <c r="D13" s="8" t="s">
         <v>8</v>
@@ -2108,7 +2108,7 @@
       <c r="AS13" s="22"/>
     </row>
     <row r="14" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="97"/>
+      <c r="B14" s="100"/>
       <c r="C14" s="81" t="s">
         <v>46</v>
       </c>
@@ -2160,7 +2160,7 @@
       <c r="AS14" s="22"/>
     </row>
     <row r="15" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="98"/>
+      <c r="B15" s="101"/>
       <c r="C15" s="82"/>
       <c r="D15" s="5" t="s">
         <v>8</v>
@@ -2210,10 +2210,10 @@
       <c r="AS15" s="23"/>
     </row>
     <row r="16" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="96" t="s">
+      <c r="B16" s="99" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="99" t="s">
+      <c r="C16" s="102" t="s">
         <v>9</v>
       </c>
       <c r="D16" s="10" t="s">
@@ -2264,7 +2264,7 @@
       <c r="AS16" s="27"/>
     </row>
     <row r="17" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="97"/>
+      <c r="B17" s="100"/>
       <c r="C17" s="81"/>
       <c r="D17" s="8" t="s">
         <v>8</v>
@@ -2314,7 +2314,7 @@
       <c r="AS17" s="22"/>
     </row>
     <row r="18" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="97"/>
+      <c r="B18" s="100"/>
       <c r="C18" s="81" t="s">
         <v>10</v>
       </c>
@@ -2366,7 +2366,7 @@
       <c r="AS18" s="22"/>
     </row>
     <row r="19" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="97"/>
+      <c r="B19" s="100"/>
       <c r="C19" s="81"/>
       <c r="D19" s="8" t="s">
         <v>8</v>
@@ -2416,7 +2416,7 @@
       <c r="AS19" s="22"/>
     </row>
     <row r="20" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="97"/>
+      <c r="B20" s="100"/>
       <c r="C20" s="81" t="s">
         <v>16</v>
       </c>
@@ -2468,12 +2468,14 @@
       <c r="AS20" s="22"/>
     </row>
     <row r="21" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="97"/>
+      <c r="B21" s="100"/>
       <c r="C21" s="81"/>
       <c r="D21" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E21" s="60"/>
+      <c r="E21" s="60">
+        <v>15</v>
+      </c>
       <c r="F21" s="14"/>
       <c r="G21" s="12"/>
       <c r="H21" s="12"/>
@@ -2487,9 +2489,9 @@
       <c r="P21" s="77"/>
       <c r="Q21" s="78"/>
       <c r="R21" s="76"/>
-      <c r="S21" s="13"/>
-      <c r="T21" s="13"/>
-      <c r="U21" s="22"/>
+      <c r="S21" s="77"/>
+      <c r="T21" s="77"/>
+      <c r="U21" s="78"/>
       <c r="V21" s="33"/>
       <c r="W21" s="13"/>
       <c r="X21" s="13"/>
@@ -2516,7 +2518,7 @@
       <c r="AS21" s="22"/>
     </row>
     <row r="22" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="97"/>
+      <c r="B22" s="100"/>
       <c r="C22" s="81" t="s">
         <v>17</v>
       </c>
@@ -2568,7 +2570,7 @@
       <c r="AS22" s="22"/>
     </row>
     <row r="23" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="97"/>
+      <c r="B23" s="100"/>
       <c r="C23" s="81"/>
       <c r="D23" s="8" t="s">
         <v>8</v>
@@ -2589,7 +2591,7 @@
       <c r="R23" s="33"/>
       <c r="S23" s="13"/>
       <c r="T23" s="13"/>
-      <c r="U23" s="22"/>
+      <c r="U23" s="78"/>
       <c r="V23" s="33"/>
       <c r="W23" s="13"/>
       <c r="X23" s="13"/>
@@ -2616,7 +2618,7 @@
       <c r="AS23" s="22"/>
     </row>
     <row r="24" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="97"/>
+      <c r="B24" s="100"/>
       <c r="C24" s="81" t="s">
         <v>14</v>
       </c>
@@ -2668,7 +2670,7 @@
       <c r="AS24" s="22"/>
     </row>
     <row r="25" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="97"/>
+      <c r="B25" s="100"/>
       <c r="C25" s="81"/>
       <c r="D25" s="8" t="s">
         <v>8</v>
@@ -2716,7 +2718,7 @@
       <c r="AS25" s="22"/>
     </row>
     <row r="26" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="97"/>
+      <c r="B26" s="100"/>
       <c r="C26" s="81" t="s">
         <v>15</v>
       </c>
@@ -2768,7 +2770,7 @@
       <c r="AS26" s="22"/>
     </row>
     <row r="27" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="98"/>
+      <c r="B27" s="101"/>
       <c r="C27" s="82"/>
       <c r="D27" s="5" t="s">
         <v>8</v>
@@ -2816,7 +2818,7 @@
       <c r="AS27" s="23"/>
     </row>
     <row r="28" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="97" t="s">
+      <c r="B28" s="100" t="s">
         <v>18</v>
       </c>
       <c r="C28" s="81" t="s">
@@ -2870,7 +2872,7 @@
       <c r="AS28" s="27"/>
     </row>
     <row r="29" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="97"/>
+      <c r="B29" s="100"/>
       <c r="C29" s="81"/>
       <c r="D29" s="8" t="s">
         <v>8</v>
@@ -2918,7 +2920,7 @@
       <c r="AS29" s="22"/>
     </row>
     <row r="30" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="97"/>
+      <c r="B30" s="100"/>
       <c r="C30" s="81" t="s">
         <v>53</v>
       </c>
@@ -2970,7 +2972,7 @@
       <c r="AS30" s="22"/>
     </row>
     <row r="31" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="97"/>
+      <c r="B31" s="100"/>
       <c r="C31" s="81"/>
       <c r="D31" s="4" t="s">
         <v>8</v>
@@ -3018,7 +3020,7 @@
       <c r="AS31" s="23"/>
     </row>
     <row r="32" spans="2:45" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="102" t="s">
+      <c r="B32" s="105" t="s">
         <v>11</v>
       </c>
       <c r="C32" s="44"/>
@@ -3047,31 +3049,31 @@
       <c r="U32" s="44"/>
       <c r="V32" s="44"/>
       <c r="W32" s="44"/>
-      <c r="X32" s="100"/>
-      <c r="Y32" s="100"/>
-      <c r="Z32" s="100"/>
-      <c r="AA32" s="100"/>
-      <c r="AB32" s="100"/>
-      <c r="AC32" s="100"/>
-      <c r="AD32" s="100"/>
-      <c r="AE32" s="100"/>
-      <c r="AF32" s="100"/>
-      <c r="AG32" s="100"/>
-      <c r="AH32" s="100"/>
-      <c r="AI32" s="100"/>
-      <c r="AJ32" s="100"/>
-      <c r="AK32" s="100"/>
-      <c r="AL32" s="100"/>
-      <c r="AM32" s="100"/>
-      <c r="AN32" s="100"/>
-      <c r="AO32" s="100"/>
-      <c r="AP32" s="100"/>
-      <c r="AQ32" s="100"/>
-      <c r="AR32" s="100"/>
-      <c r="AS32" s="101"/>
+      <c r="X32" s="103"/>
+      <c r="Y32" s="103"/>
+      <c r="Z32" s="103"/>
+      <c r="AA32" s="103"/>
+      <c r="AB32" s="103"/>
+      <c r="AC32" s="103"/>
+      <c r="AD32" s="103"/>
+      <c r="AE32" s="103"/>
+      <c r="AF32" s="103"/>
+      <c r="AG32" s="103"/>
+      <c r="AH32" s="103"/>
+      <c r="AI32" s="103"/>
+      <c r="AJ32" s="103"/>
+      <c r="AK32" s="103"/>
+      <c r="AL32" s="103"/>
+      <c r="AM32" s="103"/>
+      <c r="AN32" s="103"/>
+      <c r="AO32" s="103"/>
+      <c r="AP32" s="103"/>
+      <c r="AQ32" s="103"/>
+      <c r="AR32" s="103"/>
+      <c r="AS32" s="104"/>
     </row>
     <row r="33" spans="2:45" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="102"/>
+      <c r="B33" s="105"/>
       <c r="C33" s="44"/>
       <c r="D33" s="68" t="s">
         <v>8</v>
@@ -3119,7 +3121,7 @@
       <c r="AS33" s="48"/>
     </row>
     <row r="34" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="97" t="s">
+      <c r="B34" s="100" t="s">
         <v>19</v>
       </c>
       <c r="C34" s="81" t="s">
@@ -3173,7 +3175,7 @@
       <c r="AS34" s="21"/>
     </row>
     <row r="35" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="97"/>
+      <c r="B35" s="100"/>
       <c r="C35" s="81"/>
       <c r="D35" s="8" t="s">
         <v>8</v>
@@ -3221,8 +3223,8 @@
       <c r="AS35" s="22"/>
     </row>
     <row r="36" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="97"/>
-      <c r="C36" s="95" t="s">
+      <c r="B36" s="100"/>
+      <c r="C36" s="98" t="s">
         <v>50</v>
       </c>
       <c r="D36" s="11" t="s">
@@ -3273,8 +3275,8 @@
       <c r="AS36" s="22"/>
     </row>
     <row r="37" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="97"/>
-      <c r="C37" s="95"/>
+      <c r="B37" s="100"/>
+      <c r="C37" s="98"/>
       <c r="D37" s="8" t="s">
         <v>8</v>
       </c>
@@ -3321,7 +3323,7 @@
       <c r="AS37" s="22"/>
     </row>
     <row r="38" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="97"/>
+      <c r="B38" s="100"/>
       <c r="C38" s="81" t="s">
         <v>20</v>
       </c>
@@ -3373,7 +3375,7 @@
       <c r="AS38" s="22"/>
     </row>
     <row r="39" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="97"/>
+      <c r="B39" s="100"/>
       <c r="C39" s="81"/>
       <c r="D39" s="8" t="s">
         <v>8</v>
@@ -3421,7 +3423,7 @@
       <c r="AS39" s="22"/>
     </row>
     <row r="40" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="97"/>
+      <c r="B40" s="100"/>
       <c r="C40" s="81" t="s">
         <v>21</v>
       </c>
@@ -3473,7 +3475,7 @@
       <c r="AS40" s="22"/>
     </row>
     <row r="41" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="98"/>
+      <c r="B41" s="101"/>
       <c r="C41" s="82"/>
       <c r="D41" s="5" t="s">
         <v>8</v>
@@ -3521,10 +3523,10 @@
       <c r="AS41" s="23"/>
     </row>
     <row r="42" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="96" t="s">
+      <c r="B42" s="99" t="s">
         <v>22</v>
       </c>
-      <c r="C42" s="99" t="s">
+      <c r="C42" s="102" t="s">
         <v>23</v>
       </c>
       <c r="D42" s="10" t="s">
@@ -3575,7 +3577,7 @@
       <c r="AS42" s="27"/>
     </row>
     <row r="43" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="97"/>
+      <c r="B43" s="100"/>
       <c r="C43" s="81"/>
       <c r="D43" s="8" t="s">
         <v>8</v>
@@ -3623,7 +3625,7 @@
       <c r="AS43" s="22"/>
     </row>
     <row r="44" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="97"/>
+      <c r="B44" s="100"/>
       <c r="C44" s="81" t="s">
         <v>24</v>
       </c>
@@ -3675,7 +3677,7 @@
       <c r="AS44" s="22"/>
     </row>
     <row r="45" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="97"/>
+      <c r="B45" s="100"/>
       <c r="C45" s="81"/>
       <c r="D45" s="8" t="s">
         <v>8</v>
@@ -3723,7 +3725,7 @@
       <c r="AS45" s="22"/>
     </row>
     <row r="46" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="97"/>
+      <c r="B46" s="100"/>
       <c r="C46" s="81" t="s">
         <v>51</v>
       </c>
@@ -3775,7 +3777,7 @@
       <c r="AS46" s="22"/>
     </row>
     <row r="47" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="98"/>
+      <c r="B47" s="101"/>
       <c r="C47" s="82"/>
       <c r="D47" s="5" t="s">
         <v>8</v>
@@ -3823,10 +3825,10 @@
       <c r="AS47" s="23"/>
     </row>
     <row r="48" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="96" t="s">
+      <c r="B48" s="99" t="s">
         <v>18</v>
       </c>
-      <c r="C48" s="99" t="s">
+      <c r="C48" s="102" t="s">
         <v>25</v>
       </c>
       <c r="D48" s="10" t="s">
@@ -3877,7 +3879,7 @@
       <c r="AS48" s="27"/>
     </row>
     <row r="49" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="97"/>
+      <c r="B49" s="100"/>
       <c r="C49" s="81"/>
       <c r="D49" s="8" t="s">
         <v>8</v>
@@ -3925,7 +3927,7 @@
       <c r="AS49" s="22"/>
     </row>
     <row r="50" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="97"/>
+      <c r="B50" s="100"/>
       <c r="C50" s="81" t="s">
         <v>21</v>
       </c>
@@ -3977,7 +3979,7 @@
       <c r="AS50" s="31"/>
     </row>
     <row r="51" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="98"/>
+      <c r="B51" s="101"/>
       <c r="C51" s="82"/>
       <c r="D51" s="5" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Implementierungsphase abgeschlossen, Doku begonnen
Closing #9 & Closing #21 & mehr oder weniger #19 begonnen/gemacht

- Letzte, kleinere Verbesserungen an der App vorgenommen.
- Performance und Code start verbessert.
=> Implementierungsphase abgeschlossen
- Doku begonnen (2 Kapitel fertig, 2 weitere angefangen)
=> Zeitplan leicht angepasst, da es keinen Sinn macht die Kurzfassung als ersten zu schreiben etc.
</commit_message>
<xml_diff>
--- a/docs/ZeitplanIST.xlsx
+++ b/docs/ZeitplanIST.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mail\Code\pelan\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DD0C2F1-77C0-484A-AC25-255A4583DF79}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28B25DC3-01E7-435E-9812-15243B9E96F8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="41235" yWindow="6060" windowWidth="20355" windowHeight="12765" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="57">
   <si>
     <t>Zeitplan</t>
   </si>
@@ -89,9 +89,6 @@
     <t>Abschliessende Optimierungen</t>
   </si>
   <si>
-    <t>Erster Teil</t>
-  </si>
-  <si>
     <t>Abschlussbericht</t>
   </si>
   <si>
@@ -179,9 +176,6 @@
     <t>Arbeitsjournal &amp; Projekt aufsetzen</t>
   </si>
   <si>
-    <t>Kurzfassung &amp; Aufgabenstellung</t>
-  </si>
-  <si>
     <t>Projektmanagement, Planung &amp; Firmenstandards</t>
   </si>
   <si>
@@ -192,6 +186,21 @@
   </si>
   <si>
     <t>Ungeplante Arbeiten</t>
+  </si>
+  <si>
+    <t>Erster Teil 2.0</t>
+  </si>
+  <si>
+    <t>Erster Teil 1.0</t>
+  </si>
+  <si>
+    <t>Kurzfassung</t>
+  </si>
+  <si>
+    <t>Aufgabenstellung &amp; Analyse</t>
+  </si>
+  <si>
+    <t>Auswertung der Aufgabenstellung</t>
   </si>
 </sst>
 </file>
@@ -268,7 +277,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="37">
+  <borders count="45">
     <border>
       <left/>
       <right/>
@@ -716,11 +725,103 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF003399"/>
+      </left>
+      <right style="hair">
+        <color rgb="FF003399"/>
+      </right>
+      <top style="hair">
+        <color rgb="FF003399"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color rgb="FF003399"/>
+      </left>
+      <right style="hair">
+        <color rgb="FF003399"/>
+      </right>
+      <top style="hair">
+        <color rgb="FF003399"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color rgb="FF003399"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF003399"/>
+      </right>
+      <top style="hair">
+        <color rgb="FF003399"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color rgb="FF003399"/>
+      </right>
+      <top style="hair">
+        <color rgb="FF003399"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF003399"/>
+      </left>
+      <right style="hair">
+        <color rgb="FF003399"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color rgb="FF003399"/>
+      </left>
+      <right style="hair">
+        <color rgb="FF003399"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color rgb="FF003399"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF003399"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color rgb="FF003399"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="136">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -848,9 +949,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -961,80 +1059,173 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1045,8 +1236,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF00A5D5"/>
       <color rgb="FF003399"/>
-      <color rgb="FF00A5D5"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1360,10 +1551,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:AS51"/>
+  <dimension ref="B2:AS55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+    <sheetView tabSelected="1" topLeftCell="C7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Y40" sqref="Y40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1380,333 +1571,333 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:45" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B2" s="95" t="s">
+      <c r="B2" s="121" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="96"/>
-      <c r="H2" s="96"/>
-      <c r="I2" s="96"/>
-      <c r="J2" s="96"/>
-      <c r="K2" s="96"/>
-      <c r="L2" s="96"/>
-      <c r="M2" s="96"/>
-      <c r="N2" s="96"/>
-      <c r="O2" s="96"/>
-      <c r="P2" s="96"/>
-      <c r="Q2" s="96"/>
-      <c r="R2" s="96"/>
-      <c r="S2" s="96"/>
-      <c r="T2" s="96"/>
-      <c r="U2" s="96"/>
-      <c r="V2" s="96"/>
-      <c r="W2" s="96"/>
-      <c r="X2" s="96"/>
-      <c r="Y2" s="96"/>
-      <c r="Z2" s="96"/>
-      <c r="AA2" s="96"/>
-      <c r="AB2" s="96"/>
-      <c r="AC2" s="96"/>
-      <c r="AD2" s="96"/>
-      <c r="AE2" s="96"/>
-      <c r="AF2" s="96"/>
-      <c r="AG2" s="96"/>
-      <c r="AH2" s="96"/>
-      <c r="AI2" s="96"/>
-      <c r="AJ2" s="96"/>
-      <c r="AK2" s="96"/>
-      <c r="AL2" s="96"/>
-      <c r="AM2" s="96"/>
-      <c r="AN2" s="96"/>
-      <c r="AO2" s="96"/>
-      <c r="AP2" s="96"/>
-      <c r="AQ2" s="96"/>
-      <c r="AR2" s="96"/>
-      <c r="AS2" s="97"/>
+      <c r="C2" s="122"/>
+      <c r="D2" s="122"/>
+      <c r="E2" s="122"/>
+      <c r="F2" s="122"/>
+      <c r="G2" s="122"/>
+      <c r="H2" s="122"/>
+      <c r="I2" s="122"/>
+      <c r="J2" s="122"/>
+      <c r="K2" s="122"/>
+      <c r="L2" s="122"/>
+      <c r="M2" s="122"/>
+      <c r="N2" s="122"/>
+      <c r="O2" s="122"/>
+      <c r="P2" s="122"/>
+      <c r="Q2" s="122"/>
+      <c r="R2" s="122"/>
+      <c r="S2" s="122"/>
+      <c r="T2" s="122"/>
+      <c r="U2" s="122"/>
+      <c r="V2" s="122"/>
+      <c r="W2" s="122"/>
+      <c r="X2" s="122"/>
+      <c r="Y2" s="122"/>
+      <c r="Z2" s="122"/>
+      <c r="AA2" s="122"/>
+      <c r="AB2" s="122"/>
+      <c r="AC2" s="122"/>
+      <c r="AD2" s="122"/>
+      <c r="AE2" s="122"/>
+      <c r="AF2" s="122"/>
+      <c r="AG2" s="122"/>
+      <c r="AH2" s="122"/>
+      <c r="AI2" s="122"/>
+      <c r="AJ2" s="122"/>
+      <c r="AK2" s="122"/>
+      <c r="AL2" s="122"/>
+      <c r="AM2" s="122"/>
+      <c r="AN2" s="122"/>
+      <c r="AO2" s="122"/>
+      <c r="AP2" s="122"/>
+      <c r="AQ2" s="122"/>
+      <c r="AR2" s="122"/>
+      <c r="AS2" s="123"/>
     </row>
     <row r="3" spans="2:45" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="92" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" s="93"/>
-      <c r="D3" s="84" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="86"/>
-      <c r="F3" s="84" t="s">
+      <c r="B3" s="132" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="133"/>
+      <c r="D3" s="124" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="126"/>
+      <c r="F3" s="124" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="86"/>
-      <c r="J3" s="84" t="s">
+      <c r="G3" s="125"/>
+      <c r="H3" s="125"/>
+      <c r="I3" s="126"/>
+      <c r="J3" s="124" t="s">
+        <v>35</v>
+      </c>
+      <c r="K3" s="125"/>
+      <c r="L3" s="125"/>
+      <c r="M3" s="126"/>
+      <c r="N3" s="124" t="s">
         <v>36</v>
       </c>
-      <c r="K3" s="85"/>
-      <c r="L3" s="85"/>
-      <c r="M3" s="86"/>
-      <c r="N3" s="84" t="s">
+      <c r="O3" s="125"/>
+      <c r="P3" s="125"/>
+      <c r="Q3" s="126"/>
+      <c r="R3" s="124" t="s">
         <v>37</v>
       </c>
-      <c r="O3" s="85"/>
-      <c r="P3" s="85"/>
-      <c r="Q3" s="86"/>
-      <c r="R3" s="84" t="s">
+      <c r="S3" s="125"/>
+      <c r="T3" s="125"/>
+      <c r="U3" s="126"/>
+      <c r="V3" s="124" t="s">
         <v>38</v>
       </c>
-      <c r="S3" s="85"/>
-      <c r="T3" s="85"/>
-      <c r="U3" s="86"/>
-      <c r="V3" s="84" t="s">
+      <c r="W3" s="125"/>
+      <c r="X3" s="125"/>
+      <c r="Y3" s="126"/>
+      <c r="Z3" s="124" t="s">
         <v>39</v>
       </c>
-      <c r="W3" s="85"/>
-      <c r="X3" s="85"/>
-      <c r="Y3" s="86"/>
-      <c r="Z3" s="84" t="s">
+      <c r="AA3" s="125"/>
+      <c r="AB3" s="125"/>
+      <c r="AC3" s="126"/>
+      <c r="AD3" s="124" t="s">
         <v>40</v>
       </c>
-      <c r="AA3" s="85"/>
-      <c r="AB3" s="85"/>
-      <c r="AC3" s="86"/>
-      <c r="AD3" s="84" t="s">
+      <c r="AE3" s="125"/>
+      <c r="AF3" s="125"/>
+      <c r="AG3" s="126"/>
+      <c r="AH3" s="124" t="s">
         <v>41</v>
       </c>
-      <c r="AE3" s="85"/>
-      <c r="AF3" s="85"/>
-      <c r="AG3" s="86"/>
-      <c r="AH3" s="84" t="s">
+      <c r="AI3" s="125"/>
+      <c r="AJ3" s="125"/>
+      <c r="AK3" s="126"/>
+      <c r="AL3" s="124" t="s">
         <v>42</v>
       </c>
-      <c r="AI3" s="85"/>
-      <c r="AJ3" s="85"/>
-      <c r="AK3" s="86"/>
-      <c r="AL3" s="84" t="s">
+      <c r="AM3" s="125"/>
+      <c r="AN3" s="125"/>
+      <c r="AO3" s="126"/>
+      <c r="AP3" s="124" t="s">
         <v>43</v>
       </c>
-      <c r="AM3" s="85"/>
-      <c r="AN3" s="85"/>
-      <c r="AO3" s="86"/>
-      <c r="AP3" s="84" t="s">
-        <v>44</v>
-      </c>
-      <c r="AQ3" s="85"/>
-      <c r="AR3" s="85"/>
-      <c r="AS3" s="86"/>
+      <c r="AQ3" s="125"/>
+      <c r="AR3" s="125"/>
+      <c r="AS3" s="126"/>
     </row>
     <row r="4" spans="2:45" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="92"/>
-      <c r="C4" s="93"/>
-      <c r="D4" s="87"/>
-      <c r="E4" s="89"/>
-      <c r="F4" s="87" t="s">
+      <c r="B4" s="132"/>
+      <c r="C4" s="133"/>
+      <c r="D4" s="127"/>
+      <c r="E4" s="129"/>
+      <c r="F4" s="127" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="128"/>
+      <c r="H4" s="128"/>
+      <c r="I4" s="129"/>
+      <c r="J4" s="127" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="88"/>
-      <c r="H4" s="88"/>
-      <c r="I4" s="89"/>
-      <c r="J4" s="87" t="s">
+      <c r="K4" s="128"/>
+      <c r="L4" s="128"/>
+      <c r="M4" s="129"/>
+      <c r="N4" s="127" t="s">
         <v>27</v>
       </c>
-      <c r="K4" s="88"/>
-      <c r="L4" s="88"/>
-      <c r="M4" s="89"/>
-      <c r="N4" s="87" t="s">
+      <c r="O4" s="128"/>
+      <c r="P4" s="128"/>
+      <c r="Q4" s="129"/>
+      <c r="R4" s="127" t="s">
         <v>28</v>
       </c>
-      <c r="O4" s="88"/>
-      <c r="P4" s="88"/>
-      <c r="Q4" s="89"/>
-      <c r="R4" s="87" t="s">
+      <c r="S4" s="128"/>
+      <c r="T4" s="128"/>
+      <c r="U4" s="129"/>
+      <c r="V4" s="127" t="s">
         <v>29</v>
       </c>
-      <c r="S4" s="88"/>
-      <c r="T4" s="88"/>
-      <c r="U4" s="89"/>
-      <c r="V4" s="87" t="s">
+      <c r="W4" s="128"/>
+      <c r="X4" s="128"/>
+      <c r="Y4" s="129"/>
+      <c r="Z4" s="127" t="s">
         <v>30</v>
       </c>
-      <c r="W4" s="88"/>
-      <c r="X4" s="88"/>
-      <c r="Y4" s="89"/>
-      <c r="Z4" s="87" t="s">
+      <c r="AA4" s="128"/>
+      <c r="AB4" s="128"/>
+      <c r="AC4" s="129"/>
+      <c r="AD4" s="127" t="s">
         <v>31</v>
       </c>
-      <c r="AA4" s="88"/>
-      <c r="AB4" s="88"/>
-      <c r="AC4" s="89"/>
-      <c r="AD4" s="87" t="s">
+      <c r="AE4" s="128"/>
+      <c r="AF4" s="128"/>
+      <c r="AG4" s="129"/>
+      <c r="AH4" s="127" t="s">
         <v>32</v>
       </c>
-      <c r="AE4" s="88"/>
-      <c r="AF4" s="88"/>
-      <c r="AG4" s="89"/>
-      <c r="AH4" s="87" t="s">
+      <c r="AI4" s="128"/>
+      <c r="AJ4" s="128"/>
+      <c r="AK4" s="129"/>
+      <c r="AL4" s="127" t="s">
         <v>33</v>
       </c>
-      <c r="AI4" s="88"/>
-      <c r="AJ4" s="88"/>
-      <c r="AK4" s="89"/>
-      <c r="AL4" s="87" t="s">
+      <c r="AM4" s="128"/>
+      <c r="AN4" s="128"/>
+      <c r="AO4" s="129"/>
+      <c r="AP4" s="127" t="s">
         <v>34</v>
       </c>
-      <c r="AM4" s="88"/>
-      <c r="AN4" s="88"/>
-      <c r="AO4" s="89"/>
-      <c r="AP4" s="87" t="s">
-        <v>35</v>
-      </c>
-      <c r="AQ4" s="88"/>
-      <c r="AR4" s="88"/>
-      <c r="AS4" s="89"/>
+      <c r="AQ4" s="128"/>
+      <c r="AR4" s="128"/>
+      <c r="AS4" s="129"/>
     </row>
     <row r="5" spans="2:45" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="90" t="s">
+      <c r="B5" s="130" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="91"/>
-      <c r="D5" s="94" t="s">
+      <c r="C5" s="131"/>
+      <c r="D5" s="134" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="91"/>
-      <c r="F5" s="45">
-        <v>2</v>
-      </c>
-      <c r="G5" s="47">
-        <v>2</v>
-      </c>
-      <c r="H5" s="47">
-        <v>2</v>
-      </c>
-      <c r="I5" s="46">
-        <v>2</v>
-      </c>
-      <c r="J5" s="45">
-        <v>2</v>
-      </c>
-      <c r="K5" s="47">
-        <v>2</v>
-      </c>
-      <c r="L5" s="47">
-        <v>2</v>
-      </c>
-      <c r="M5" s="46">
-        <v>2</v>
-      </c>
-      <c r="N5" s="45">
-        <v>2</v>
-      </c>
-      <c r="O5" s="47">
-        <v>2</v>
-      </c>
-      <c r="P5" s="47">
-        <v>2</v>
-      </c>
-      <c r="Q5" s="46">
-        <v>2</v>
-      </c>
-      <c r="R5" s="45">
-        <v>2</v>
-      </c>
-      <c r="S5" s="47">
-        <v>2</v>
-      </c>
-      <c r="T5" s="47">
-        <v>2</v>
-      </c>
-      <c r="U5" s="46">
-        <v>2</v>
-      </c>
-      <c r="V5" s="45">
-        <v>2</v>
-      </c>
-      <c r="W5" s="47">
-        <v>2</v>
-      </c>
-      <c r="X5" s="47">
-        <v>2</v>
-      </c>
-      <c r="Y5" s="46">
-        <v>2</v>
-      </c>
-      <c r="Z5" s="45">
-        <v>2</v>
-      </c>
-      <c r="AA5" s="47">
-        <v>2</v>
-      </c>
-      <c r="AB5" s="47">
-        <v>2</v>
-      </c>
-      <c r="AC5" s="46">
-        <v>2</v>
-      </c>
-      <c r="AD5" s="45">
-        <v>2</v>
-      </c>
-      <c r="AE5" s="47">
-        <v>2</v>
-      </c>
-      <c r="AF5" s="47">
-        <v>2</v>
-      </c>
-      <c r="AG5" s="46">
-        <v>2</v>
-      </c>
-      <c r="AH5" s="45">
-        <v>2</v>
-      </c>
-      <c r="AI5" s="47">
-        <v>2</v>
-      </c>
-      <c r="AJ5" s="47">
-        <v>2</v>
-      </c>
-      <c r="AK5" s="46">
-        <v>2</v>
-      </c>
-      <c r="AL5" s="45">
-        <v>2</v>
-      </c>
-      <c r="AM5" s="47">
-        <v>2</v>
-      </c>
-      <c r="AN5" s="47">
-        <v>2</v>
-      </c>
-      <c r="AO5" s="46">
-        <v>2</v>
-      </c>
-      <c r="AP5" s="45">
-        <v>2</v>
-      </c>
-      <c r="AQ5" s="47">
-        <v>2</v>
-      </c>
-      <c r="AR5" s="47">
-        <v>2</v>
-      </c>
-      <c r="AS5" s="46">
+      <c r="E5" s="131"/>
+      <c r="F5" s="44">
+        <v>2</v>
+      </c>
+      <c r="G5" s="46">
+        <v>2</v>
+      </c>
+      <c r="H5" s="46">
+        <v>2</v>
+      </c>
+      <c r="I5" s="45">
+        <v>2</v>
+      </c>
+      <c r="J5" s="44">
+        <v>2</v>
+      </c>
+      <c r="K5" s="46">
+        <v>2</v>
+      </c>
+      <c r="L5" s="46">
+        <v>2</v>
+      </c>
+      <c r="M5" s="45">
+        <v>2</v>
+      </c>
+      <c r="N5" s="44">
+        <v>2</v>
+      </c>
+      <c r="O5" s="46">
+        <v>2</v>
+      </c>
+      <c r="P5" s="46">
+        <v>2</v>
+      </c>
+      <c r="Q5" s="45">
+        <v>2</v>
+      </c>
+      <c r="R5" s="44">
+        <v>2</v>
+      </c>
+      <c r="S5" s="46">
+        <v>2</v>
+      </c>
+      <c r="T5" s="46">
+        <v>2</v>
+      </c>
+      <c r="U5" s="45">
+        <v>2</v>
+      </c>
+      <c r="V5" s="44">
+        <v>2</v>
+      </c>
+      <c r="W5" s="46">
+        <v>2</v>
+      </c>
+      <c r="X5" s="46">
+        <v>2</v>
+      </c>
+      <c r="Y5" s="45">
+        <v>2</v>
+      </c>
+      <c r="Z5" s="44">
+        <v>2</v>
+      </c>
+      <c r="AA5" s="46">
+        <v>2</v>
+      </c>
+      <c r="AB5" s="46">
+        <v>2</v>
+      </c>
+      <c r="AC5" s="45">
+        <v>2</v>
+      </c>
+      <c r="AD5" s="44">
+        <v>2</v>
+      </c>
+      <c r="AE5" s="46">
+        <v>2</v>
+      </c>
+      <c r="AF5" s="46">
+        <v>2</v>
+      </c>
+      <c r="AG5" s="45">
+        <v>2</v>
+      </c>
+      <c r="AH5" s="44">
+        <v>2</v>
+      </c>
+      <c r="AI5" s="46">
+        <v>2</v>
+      </c>
+      <c r="AJ5" s="46">
+        <v>2</v>
+      </c>
+      <c r="AK5" s="45">
+        <v>2</v>
+      </c>
+      <c r="AL5" s="44">
+        <v>2</v>
+      </c>
+      <c r="AM5" s="46">
+        <v>2</v>
+      </c>
+      <c r="AN5" s="46">
+        <v>2</v>
+      </c>
+      <c r="AO5" s="45">
+        <v>2</v>
+      </c>
+      <c r="AP5" s="44">
+        <v>2</v>
+      </c>
+      <c r="AQ5" s="46">
+        <v>2</v>
+      </c>
+      <c r="AR5" s="46">
+        <v>2</v>
+      </c>
+      <c r="AS5" s="45">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="2:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="83" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="81" t="s">
-        <v>48</v>
+      <c r="B6" s="135" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="113" t="s">
+        <v>47</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="57">
-        <v>2</v>
-      </c>
-      <c r="F6" s="49"/>
+      <c r="E6" s="56">
+        <v>2</v>
+      </c>
+      <c r="F6" s="48"/>
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
       <c r="I6" s="38"/>
@@ -1748,15 +1939,15 @@
       <c r="AS6" s="22"/>
     </row>
     <row r="7" spans="2:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="84"/>
-      <c r="C7" s="81"/>
+      <c r="B7" s="124"/>
+      <c r="C7" s="113"/>
       <c r="D7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="58">
+      <c r="E7" s="57">
         <v>1.5</v>
       </c>
-      <c r="F7" s="70"/>
+      <c r="F7" s="69"/>
       <c r="G7" s="19"/>
       <c r="H7" s="19"/>
       <c r="I7" s="40"/>
@@ -1798,114 +1989,114 @@
       <c r="AS7" s="23"/>
     </row>
     <row r="8" spans="2:45" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="105" t="s">
+      <c r="B8" s="119" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="44"/>
-      <c r="D8" s="67" t="s">
+      <c r="C8" s="43"/>
+      <c r="D8" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="67">
+      <c r="E8" s="66">
         <f>SUM(E10+E12+E14+E16+E18+E20+E22+E24+E26+E28+E30)</f>
         <v>34</v>
       </c>
-      <c r="F8" s="44"/>
-      <c r="G8" s="103"/>
-      <c r="H8" s="103"/>
-      <c r="I8" s="103"/>
-      <c r="J8" s="103"/>
-      <c r="K8" s="103"/>
-      <c r="L8" s="103"/>
-      <c r="M8" s="103"/>
-      <c r="N8" s="103"/>
-      <c r="O8" s="103"/>
-      <c r="P8" s="103"/>
-      <c r="Q8" s="103"/>
-      <c r="R8" s="103"/>
-      <c r="S8" s="103"/>
-      <c r="T8" s="103"/>
-      <c r="U8" s="103"/>
-      <c r="V8" s="103"/>
-      <c r="W8" s="103"/>
-      <c r="X8" s="44"/>
-      <c r="Y8" s="44"/>
-      <c r="Z8" s="44"/>
-      <c r="AA8" s="44"/>
-      <c r="AB8" s="44"/>
-      <c r="AC8" s="44"/>
-      <c r="AD8" s="44"/>
-      <c r="AE8" s="44"/>
-      <c r="AF8" s="44"/>
-      <c r="AG8" s="44"/>
-      <c r="AH8" s="44"/>
-      <c r="AI8" s="44"/>
-      <c r="AJ8" s="44"/>
-      <c r="AK8" s="44"/>
-      <c r="AL8" s="44"/>
-      <c r="AM8" s="44"/>
-      <c r="AN8" s="44"/>
-      <c r="AO8" s="44"/>
-      <c r="AP8" s="44"/>
-      <c r="AQ8" s="44"/>
-      <c r="AR8" s="44"/>
-      <c r="AS8" s="48"/>
+      <c r="F8" s="111"/>
+      <c r="G8" s="111"/>
+      <c r="H8" s="111"/>
+      <c r="I8" s="111"/>
+      <c r="J8" s="111"/>
+      <c r="K8" s="111"/>
+      <c r="L8" s="111"/>
+      <c r="M8" s="111"/>
+      <c r="N8" s="111"/>
+      <c r="O8" s="111"/>
+      <c r="P8" s="111"/>
+      <c r="Q8" s="111"/>
+      <c r="R8" s="111"/>
+      <c r="S8" s="111"/>
+      <c r="T8" s="111"/>
+      <c r="U8" s="111"/>
+      <c r="V8" s="111"/>
+      <c r="W8" s="81"/>
+      <c r="X8" s="43"/>
+      <c r="Y8" s="43"/>
+      <c r="Z8" s="43"/>
+      <c r="AA8" s="43"/>
+      <c r="AB8" s="43"/>
+      <c r="AC8" s="43"/>
+      <c r="AD8" s="43"/>
+      <c r="AE8" s="43"/>
+      <c r="AF8" s="43"/>
+      <c r="AG8" s="43"/>
+      <c r="AH8" s="43"/>
+      <c r="AI8" s="43"/>
+      <c r="AJ8" s="43"/>
+      <c r="AK8" s="43"/>
+      <c r="AL8" s="43"/>
+      <c r="AM8" s="43"/>
+      <c r="AN8" s="43"/>
+      <c r="AO8" s="43"/>
+      <c r="AP8" s="43"/>
+      <c r="AQ8" s="43"/>
+      <c r="AR8" s="43"/>
+      <c r="AS8" s="47"/>
     </row>
     <row r="9" spans="2:45" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="105"/>
-      <c r="C9" s="44"/>
-      <c r="D9" s="68" t="s">
+      <c r="B9" s="119"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="67">
+      <c r="E9" s="66">
         <f>SUM(E11+E13+E15+E17+E19+E21+E23+E25+E27+E29+E31)</f>
-        <v>28</v>
-      </c>
-      <c r="F9" s="79"/>
-      <c r="G9" s="80"/>
-      <c r="H9" s="80"/>
-      <c r="I9" s="80"/>
-      <c r="J9" s="80"/>
-      <c r="K9" s="80"/>
-      <c r="L9" s="80"/>
-      <c r="M9" s="80"/>
-      <c r="N9" s="80"/>
-      <c r="O9" s="80"/>
-      <c r="P9" s="80"/>
-      <c r="Q9" s="80"/>
-      <c r="R9" s="80"/>
-      <c r="S9" s="80"/>
-      <c r="T9" s="80"/>
-      <c r="U9" s="80"/>
-      <c r="V9" s="69"/>
-      <c r="W9" s="69"/>
-      <c r="X9" s="44"/>
-      <c r="Y9" s="44"/>
-      <c r="Z9" s="44"/>
-      <c r="AA9" s="44"/>
-      <c r="AB9" s="44"/>
-      <c r="AC9" s="44"/>
-      <c r="AD9" s="44"/>
-      <c r="AE9" s="44"/>
-      <c r="AF9" s="44"/>
-      <c r="AG9" s="44"/>
-      <c r="AH9" s="44"/>
-      <c r="AI9" s="44"/>
-      <c r="AJ9" s="44"/>
-      <c r="AK9" s="44"/>
-      <c r="AL9" s="44"/>
-      <c r="AM9" s="44"/>
-      <c r="AN9" s="44"/>
-      <c r="AO9" s="44"/>
-      <c r="AP9" s="44"/>
-      <c r="AQ9" s="44"/>
-      <c r="AR9" s="44"/>
-      <c r="AS9" s="66"/>
+        <v>34</v>
+      </c>
+      <c r="F9" s="78"/>
+      <c r="G9" s="79"/>
+      <c r="H9" s="79"/>
+      <c r="I9" s="79"/>
+      <c r="J9" s="79"/>
+      <c r="K9" s="79"/>
+      <c r="L9" s="79"/>
+      <c r="M9" s="79"/>
+      <c r="N9" s="79"/>
+      <c r="O9" s="79"/>
+      <c r="P9" s="79"/>
+      <c r="Q9" s="79"/>
+      <c r="R9" s="79"/>
+      <c r="S9" s="79"/>
+      <c r="T9" s="79"/>
+      <c r="U9" s="79"/>
+      <c r="V9" s="79"/>
+      <c r="W9" s="79"/>
+      <c r="X9" s="78"/>
+      <c r="Y9" s="43"/>
+      <c r="Z9" s="43"/>
+      <c r="AA9" s="43"/>
+      <c r="AB9" s="43"/>
+      <c r="AC9" s="43"/>
+      <c r="AD9" s="43"/>
+      <c r="AE9" s="43"/>
+      <c r="AF9" s="43"/>
+      <c r="AG9" s="43"/>
+      <c r="AH9" s="43"/>
+      <c r="AI9" s="43"/>
+      <c r="AJ9" s="43"/>
+      <c r="AK9" s="43"/>
+      <c r="AL9" s="43"/>
+      <c r="AM9" s="43"/>
+      <c r="AN9" s="43"/>
+      <c r="AO9" s="43"/>
+      <c r="AP9" s="43"/>
+      <c r="AQ9" s="43"/>
+      <c r="AR9" s="43"/>
+      <c r="AS9" s="65"/>
     </row>
     <row r="10" spans="2:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="100" t="s">
+      <c r="B10" s="114" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="81" t="s">
+      <c r="C10" s="113" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="10" t="s">
@@ -1956,16 +2147,16 @@
       <c r="AS10" s="21"/>
     </row>
     <row r="11" spans="2:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="100"/>
-      <c r="C11" s="81"/>
+      <c r="B11" s="114"/>
+      <c r="C11" s="113"/>
       <c r="D11" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="60">
+      <c r="E11" s="59">
         <v>2.5</v>
       </c>
-      <c r="F11" s="71"/>
-      <c r="G11" s="72"/>
+      <c r="F11" s="70"/>
+      <c r="G11" s="71"/>
       <c r="H11" s="12"/>
       <c r="I11" s="38"/>
       <c r="J11" s="33"/>
@@ -2006,14 +2197,14 @@
       <c r="AS11" s="22"/>
     </row>
     <row r="12" spans="2:45" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="100"/>
-      <c r="C12" s="81" t="s">
-        <v>47</v>
+      <c r="B12" s="114"/>
+      <c r="C12" s="113" t="s">
+        <v>46</v>
       </c>
       <c r="D12" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="61">
+      <c r="E12" s="60">
         <v>2</v>
       </c>
       <c r="F12" s="14"/>
@@ -2058,18 +2249,18 @@
       <c r="AS12" s="22"/>
     </row>
     <row r="13" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="100"/>
-      <c r="C13" s="81"/>
+      <c r="B13" s="114"/>
+      <c r="C13" s="113"/>
       <c r="D13" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="62">
+      <c r="E13" s="61">
         <v>3.5</v>
       </c>
       <c r="F13" s="14"/>
       <c r="G13" s="12"/>
-      <c r="H13" s="72"/>
-      <c r="I13" s="73"/>
+      <c r="H13" s="71"/>
+      <c r="I13" s="72"/>
       <c r="J13" s="33"/>
       <c r="K13" s="13"/>
       <c r="L13" s="13"/>
@@ -2108,9 +2299,9 @@
       <c r="AS13" s="22"/>
     </row>
     <row r="14" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="100"/>
-      <c r="C14" s="81" t="s">
-        <v>46</v>
+      <c r="B14" s="114"/>
+      <c r="C14" s="113" t="s">
+        <v>45</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>7</v>
@@ -2160,19 +2351,19 @@
       <c r="AS14" s="22"/>
     </row>
     <row r="15" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="101"/>
-      <c r="C15" s="82"/>
+      <c r="B15" s="118"/>
+      <c r="C15" s="116"/>
       <c r="D15" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="63">
+      <c r="E15" s="62">
         <v>1</v>
       </c>
       <c r="F15" s="18"/>
       <c r="G15" s="19"/>
       <c r="H15" s="19"/>
-      <c r="I15" s="74"/>
-      <c r="J15" s="75"/>
+      <c r="I15" s="73"/>
+      <c r="J15" s="74"/>
       <c r="K15" s="20"/>
       <c r="L15" s="20"/>
       <c r="M15" s="23"/>
@@ -2210,16 +2401,16 @@
       <c r="AS15" s="23"/>
     </row>
     <row r="16" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="99" t="s">
+      <c r="B16" s="117" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="102" t="s">
+      <c r="C16" s="115" t="s">
         <v>9</v>
       </c>
       <c r="D16" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E16" s="64">
+      <c r="E16" s="63">
         <v>4</v>
       </c>
       <c r="F16" s="24"/>
@@ -2264,20 +2455,20 @@
       <c r="AS16" s="27"/>
     </row>
     <row r="17" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="100"/>
-      <c r="C17" s="81"/>
+      <c r="B17" s="114"/>
+      <c r="C17" s="113"/>
       <c r="D17" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E17" s="60">
+      <c r="E17" s="59">
         <v>3.5</v>
       </c>
       <c r="F17" s="14"/>
       <c r="G17" s="12"/>
       <c r="H17" s="12"/>
       <c r="I17" s="38"/>
-      <c r="J17" s="76"/>
-      <c r="K17" s="77"/>
+      <c r="J17" s="75"/>
+      <c r="K17" s="76"/>
       <c r="L17" s="13"/>
       <c r="M17" s="22"/>
       <c r="N17" s="33"/>
@@ -2314,14 +2505,14 @@
       <c r="AS17" s="22"/>
     </row>
     <row r="18" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="100"/>
-      <c r="C18" s="81" t="s">
+      <c r="B18" s="114"/>
+      <c r="C18" s="113" t="s">
         <v>10</v>
       </c>
       <c r="D18" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E18" s="65">
+      <c r="E18" s="64">
         <v>2</v>
       </c>
       <c r="F18" s="14"/>
@@ -2366,12 +2557,12 @@
       <c r="AS18" s="22"/>
     </row>
     <row r="19" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="100"/>
-      <c r="C19" s="81"/>
+      <c r="B19" s="114"/>
+      <c r="C19" s="113"/>
       <c r="D19" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E19" s="60">
+      <c r="E19" s="59">
         <v>2.5</v>
       </c>
       <c r="F19" s="14"/>
@@ -2380,8 +2571,8 @@
       <c r="I19" s="38"/>
       <c r="J19" s="33"/>
       <c r="K19" s="13"/>
-      <c r="L19" s="77"/>
-      <c r="M19" s="78"/>
+      <c r="L19" s="76"/>
+      <c r="M19" s="77"/>
       <c r="N19" s="33"/>
       <c r="O19" s="13"/>
       <c r="P19" s="13"/>
@@ -2416,14 +2607,14 @@
       <c r="AS19" s="22"/>
     </row>
     <row r="20" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="100"/>
-      <c r="C20" s="81" t="s">
+      <c r="B20" s="114"/>
+      <c r="C20" s="113" t="s">
         <v>16</v>
       </c>
       <c r="D20" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E20" s="65">
+      <c r="E20" s="64">
         <v>12</v>
       </c>
       <c r="F20" s="14"/>
@@ -2468,12 +2659,12 @@
       <c r="AS20" s="22"/>
     </row>
     <row r="21" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="100"/>
-      <c r="C21" s="81"/>
+      <c r="B21" s="114"/>
+      <c r="C21" s="113"/>
       <c r="D21" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E21" s="60">
+      <c r="E21" s="59">
         <v>15</v>
       </c>
       <c r="F21" s="14"/>
@@ -2484,14 +2675,14 @@
       <c r="K21" s="13"/>
       <c r="L21" s="13"/>
       <c r="M21" s="22"/>
-      <c r="N21" s="76"/>
-      <c r="O21" s="77"/>
-      <c r="P21" s="77"/>
-      <c r="Q21" s="78"/>
-      <c r="R21" s="76"/>
-      <c r="S21" s="77"/>
-      <c r="T21" s="77"/>
-      <c r="U21" s="78"/>
+      <c r="N21" s="75"/>
+      <c r="O21" s="76"/>
+      <c r="P21" s="76"/>
+      <c r="Q21" s="77"/>
+      <c r="R21" s="75"/>
+      <c r="S21" s="76"/>
+      <c r="T21" s="76"/>
+      <c r="U21" s="77"/>
       <c r="V21" s="33"/>
       <c r="W21" s="13"/>
       <c r="X21" s="13"/>
@@ -2518,14 +2709,14 @@
       <c r="AS21" s="22"/>
     </row>
     <row r="22" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="100"/>
-      <c r="C22" s="81" t="s">
+      <c r="B22" s="114"/>
+      <c r="C22" s="113" t="s">
         <v>17</v>
       </c>
       <c r="D22" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E22" s="65">
+      <c r="E22" s="64">
         <v>2</v>
       </c>
       <c r="F22" s="14"/>
@@ -2540,7 +2731,7 @@
       <c r="O22" s="13"/>
       <c r="P22" s="13"/>
       <c r="Q22" s="22"/>
-      <c r="R22" s="50"/>
+      <c r="R22" s="49"/>
       <c r="S22" s="13"/>
       <c r="T22" s="30"/>
       <c r="U22" s="22"/>
@@ -2570,12 +2761,14 @@
       <c r="AS22" s="22"/>
     </row>
     <row r="23" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="100"/>
-      <c r="C23" s="81"/>
+      <c r="B23" s="114"/>
+      <c r="C23" s="113"/>
       <c r="D23" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E23" s="60"/>
+      <c r="E23" s="59">
+        <v>2</v>
+      </c>
       <c r="F23" s="14"/>
       <c r="G23" s="12"/>
       <c r="H23" s="12"/>
@@ -2591,8 +2784,8 @@
       <c r="R23" s="33"/>
       <c r="S23" s="13"/>
       <c r="T23" s="13"/>
-      <c r="U23" s="78"/>
-      <c r="V23" s="33"/>
+      <c r="U23" s="77"/>
+      <c r="V23" s="75"/>
       <c r="W23" s="13"/>
       <c r="X23" s="13"/>
       <c r="Y23" s="22"/>
@@ -2618,14 +2811,14 @@
       <c r="AS23" s="22"/>
     </row>
     <row r="24" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="100"/>
-      <c r="C24" s="81" t="s">
+      <c r="B24" s="114"/>
+      <c r="C24" s="113" t="s">
         <v>14</v>
       </c>
       <c r="D24" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E24" s="65">
+      <c r="E24" s="64">
         <v>2</v>
       </c>
       <c r="F24" s="14"/>
@@ -2641,7 +2834,7 @@
       <c r="P24" s="13"/>
       <c r="Q24" s="22"/>
       <c r="R24" s="33"/>
-      <c r="S24" s="51"/>
+      <c r="S24" s="50"/>
       <c r="T24" s="13"/>
       <c r="U24" s="31"/>
       <c r="V24" s="33"/>
@@ -2670,12 +2863,14 @@
       <c r="AS24" s="22"/>
     </row>
     <row r="25" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="100"/>
-      <c r="C25" s="81"/>
+      <c r="B25" s="114"/>
+      <c r="C25" s="113"/>
       <c r="D25" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E25" s="60"/>
+      <c r="E25" s="59">
+        <v>1</v>
+      </c>
       <c r="F25" s="14"/>
       <c r="G25" s="12"/>
       <c r="H25" s="12"/>
@@ -2692,7 +2887,7 @@
       <c r="S25" s="13"/>
       <c r="T25" s="13"/>
       <c r="U25" s="22"/>
-      <c r="V25" s="33"/>
+      <c r="V25" s="75"/>
       <c r="W25" s="13"/>
       <c r="X25" s="13"/>
       <c r="Y25" s="22"/>
@@ -2718,8 +2913,8 @@
       <c r="AS25" s="22"/>
     </row>
     <row r="26" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="100"/>
-      <c r="C26" s="81" t="s">
+      <c r="B26" s="114"/>
+      <c r="C26" s="113" t="s">
         <v>15</v>
       </c>
       <c r="D26" s="4" t="s">
@@ -2742,7 +2937,7 @@
       <c r="Q26" s="22"/>
       <c r="R26" s="33"/>
       <c r="S26" s="13"/>
-      <c r="T26" s="51"/>
+      <c r="T26" s="50"/>
       <c r="U26" s="22"/>
       <c r="V26" s="42"/>
       <c r="W26" s="13"/>
@@ -2770,12 +2965,14 @@
       <c r="AS26" s="22"/>
     </row>
     <row r="27" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="101"/>
-      <c r="C27" s="82"/>
+      <c r="B27" s="118"/>
+      <c r="C27" s="116"/>
       <c r="D27" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E27" s="63"/>
+      <c r="E27" s="62">
+        <v>1</v>
+      </c>
       <c r="F27" s="18"/>
       <c r="G27" s="19"/>
       <c r="H27" s="19"/>
@@ -2792,8 +2989,8 @@
       <c r="S27" s="20"/>
       <c r="T27" s="20"/>
       <c r="U27" s="23"/>
-      <c r="V27" s="34"/>
-      <c r="W27" s="20"/>
+      <c r="V27" s="74"/>
+      <c r="W27" s="80"/>
       <c r="X27" s="20"/>
       <c r="Y27" s="23"/>
       <c r="Z27" s="34"/>
@@ -2818,11 +3015,11 @@
       <c r="AS27" s="23"/>
     </row>
     <row r="28" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="100" t="s">
+      <c r="B28" s="114" t="s">
         <v>18</v>
       </c>
-      <c r="C28" s="81" t="s">
-        <v>52</v>
+      <c r="C28" s="113" t="s">
+        <v>50</v>
       </c>
       <c r="D28" s="7" t="s">
         <v>7</v>
@@ -2845,7 +3042,7 @@
       <c r="R28" s="36"/>
       <c r="S28" s="26"/>
       <c r="T28" s="26"/>
-      <c r="U28" s="52"/>
+      <c r="U28" s="51"/>
       <c r="V28" s="36"/>
       <c r="W28" s="29"/>
       <c r="X28" s="26"/>
@@ -2872,12 +3069,14 @@
       <c r="AS28" s="27"/>
     </row>
     <row r="29" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="100"/>
-      <c r="C29" s="81"/>
+      <c r="B29" s="114"/>
+      <c r="C29" s="113"/>
       <c r="D29" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E29" s="60"/>
+      <c r="E29" s="59">
+        <v>1</v>
+      </c>
       <c r="F29" s="14"/>
       <c r="G29" s="12"/>
       <c r="H29" s="12"/>
@@ -2895,8 +3094,8 @@
       <c r="T29" s="13"/>
       <c r="U29" s="22"/>
       <c r="V29" s="33"/>
-      <c r="W29" s="13"/>
-      <c r="X29" s="13"/>
+      <c r="W29" s="76"/>
+      <c r="X29" s="76"/>
       <c r="Y29" s="22"/>
       <c r="Z29" s="33"/>
       <c r="AA29" s="13"/>
@@ -2920,9 +3119,9 @@
       <c r="AS29" s="22"/>
     </row>
     <row r="30" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="100"/>
-      <c r="C30" s="81" t="s">
-        <v>53</v>
+      <c r="B30" s="114"/>
+      <c r="C30" s="113" t="s">
+        <v>51</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>7</v>
@@ -2945,7 +3144,7 @@
       <c r="R30" s="33"/>
       <c r="S30" s="13"/>
       <c r="T30" s="13"/>
-      <c r="U30" s="53"/>
+      <c r="U30" s="52"/>
       <c r="V30" s="33"/>
       <c r="W30" s="30"/>
       <c r="X30" s="13"/>
@@ -2972,12 +3171,14 @@
       <c r="AS30" s="22"/>
     </row>
     <row r="31" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="100"/>
-      <c r="C31" s="81"/>
+      <c r="B31" s="114"/>
+      <c r="C31" s="113"/>
       <c r="D31" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E31" s="2"/>
+      <c r="E31" s="2">
+        <v>1</v>
+      </c>
       <c r="F31" s="18"/>
       <c r="G31" s="19"/>
       <c r="H31" s="19"/>
@@ -2995,8 +3196,8 @@
       <c r="T31" s="20"/>
       <c r="U31" s="23"/>
       <c r="V31" s="34"/>
-      <c r="W31" s="20"/>
-      <c r="X31" s="20"/>
+      <c r="W31" s="80"/>
+      <c r="X31" s="80"/>
       <c r="Y31" s="23"/>
       <c r="Z31" s="34"/>
       <c r="AA31" s="20"/>
@@ -3020,112 +3221,112 @@
       <c r="AS31" s="23"/>
     </row>
     <row r="32" spans="2:45" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="105" t="s">
+      <c r="B32" s="119" t="s">
         <v>11</v>
       </c>
-      <c r="C32" s="44"/>
-      <c r="D32" s="67" t="s">
+      <c r="C32" s="43"/>
+      <c r="D32" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="E32" s="67">
-        <f>SUM(E34+E36+E38+E40+E42+E44+E46+E48+E50)</f>
+      <c r="E32" s="66">
+        <f>SUM(E34+E36+E38+E40+E42+E44+E46+E52+E54+E48+E50)</f>
         <v>44</v>
       </c>
-      <c r="F32" s="44"/>
-      <c r="G32" s="44"/>
-      <c r="H32" s="44"/>
-      <c r="I32" s="44"/>
-      <c r="J32" s="44"/>
-      <c r="K32" s="44"/>
-      <c r="L32" s="44"/>
-      <c r="M32" s="44"/>
-      <c r="N32" s="44"/>
-      <c r="O32" s="44"/>
-      <c r="P32" s="44"/>
-      <c r="Q32" s="44"/>
-      <c r="R32" s="44"/>
-      <c r="S32" s="44"/>
-      <c r="T32" s="44"/>
-      <c r="U32" s="44"/>
-      <c r="V32" s="44"/>
-      <c r="W32" s="44"/>
-      <c r="X32" s="103"/>
-      <c r="Y32" s="103"/>
-      <c r="Z32" s="103"/>
-      <c r="AA32" s="103"/>
-      <c r="AB32" s="103"/>
-      <c r="AC32" s="103"/>
-      <c r="AD32" s="103"/>
-      <c r="AE32" s="103"/>
-      <c r="AF32" s="103"/>
-      <c r="AG32" s="103"/>
-      <c r="AH32" s="103"/>
-      <c r="AI32" s="103"/>
-      <c r="AJ32" s="103"/>
-      <c r="AK32" s="103"/>
-      <c r="AL32" s="103"/>
-      <c r="AM32" s="103"/>
-      <c r="AN32" s="103"/>
-      <c r="AO32" s="103"/>
-      <c r="AP32" s="103"/>
-      <c r="AQ32" s="103"/>
-      <c r="AR32" s="103"/>
-      <c r="AS32" s="104"/>
+      <c r="F32" s="43"/>
+      <c r="G32" s="43"/>
+      <c r="H32" s="43"/>
+      <c r="I32" s="43"/>
+      <c r="J32" s="43"/>
+      <c r="K32" s="43"/>
+      <c r="L32" s="43"/>
+      <c r="M32" s="43"/>
+      <c r="N32" s="43"/>
+      <c r="O32" s="43"/>
+      <c r="P32" s="43"/>
+      <c r="Q32" s="43"/>
+      <c r="R32" s="43"/>
+      <c r="S32" s="43"/>
+      <c r="T32" s="43"/>
+      <c r="U32" s="43"/>
+      <c r="V32" s="43"/>
+      <c r="W32" s="43"/>
+      <c r="X32" s="111"/>
+      <c r="Y32" s="111"/>
+      <c r="Z32" s="111"/>
+      <c r="AA32" s="111"/>
+      <c r="AB32" s="111"/>
+      <c r="AC32" s="111"/>
+      <c r="AD32" s="111"/>
+      <c r="AE32" s="111"/>
+      <c r="AF32" s="111"/>
+      <c r="AG32" s="111"/>
+      <c r="AH32" s="111"/>
+      <c r="AI32" s="111"/>
+      <c r="AJ32" s="111"/>
+      <c r="AK32" s="111"/>
+      <c r="AL32" s="111"/>
+      <c r="AM32" s="111"/>
+      <c r="AN32" s="111"/>
+      <c r="AO32" s="111"/>
+      <c r="AP32" s="111"/>
+      <c r="AQ32" s="111"/>
+      <c r="AR32" s="111"/>
+      <c r="AS32" s="112"/>
     </row>
     <row r="33" spans="2:45" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="105"/>
-      <c r="C33" s="44"/>
-      <c r="D33" s="68" t="s">
+      <c r="B33" s="119"/>
+      <c r="C33" s="43"/>
+      <c r="D33" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="E33" s="59"/>
-      <c r="F33" s="44"/>
-      <c r="G33" s="44"/>
-      <c r="H33" s="44"/>
-      <c r="I33" s="44"/>
-      <c r="J33" s="44"/>
-      <c r="K33" s="44"/>
-      <c r="L33" s="44"/>
-      <c r="M33" s="44"/>
-      <c r="N33" s="44"/>
-      <c r="O33" s="44"/>
-      <c r="P33" s="44"/>
-      <c r="Q33" s="44"/>
-      <c r="R33" s="44"/>
-      <c r="S33" s="44"/>
-      <c r="T33" s="44"/>
-      <c r="U33" s="44"/>
-      <c r="V33" s="44"/>
-      <c r="W33" s="44"/>
-      <c r="X33" s="69"/>
-      <c r="Y33" s="69"/>
-      <c r="Z33" s="69"/>
-      <c r="AA33" s="69"/>
-      <c r="AB33" s="69"/>
-      <c r="AC33" s="69"/>
-      <c r="AD33" s="69"/>
-      <c r="AE33" s="69"/>
-      <c r="AF33" s="69"/>
-      <c r="AG33" s="69"/>
-      <c r="AH33" s="69"/>
-      <c r="AI33" s="69"/>
-      <c r="AJ33" s="69"/>
-      <c r="AK33" s="69"/>
-      <c r="AL33" s="69"/>
-      <c r="AM33" s="69"/>
-      <c r="AN33" s="69"/>
-      <c r="AO33" s="69"/>
-      <c r="AP33" s="69"/>
-      <c r="AQ33" s="69"/>
-      <c r="AR33" s="69"/>
-      <c r="AS33" s="48"/>
+      <c r="E33" s="58"/>
+      <c r="F33" s="43"/>
+      <c r="G33" s="43"/>
+      <c r="H33" s="43"/>
+      <c r="I33" s="43"/>
+      <c r="J33" s="43"/>
+      <c r="K33" s="43"/>
+      <c r="L33" s="43"/>
+      <c r="M33" s="43"/>
+      <c r="N33" s="43"/>
+      <c r="O33" s="43"/>
+      <c r="P33" s="43"/>
+      <c r="Q33" s="43"/>
+      <c r="R33" s="43"/>
+      <c r="S33" s="43"/>
+      <c r="T33" s="43"/>
+      <c r="U33" s="43"/>
+      <c r="V33" s="43"/>
+      <c r="W33" s="43"/>
+      <c r="X33" s="79"/>
+      <c r="Y33" s="79"/>
+      <c r="Z33" s="68"/>
+      <c r="AA33" s="68"/>
+      <c r="AB33" s="68"/>
+      <c r="AC33" s="68"/>
+      <c r="AD33" s="68"/>
+      <c r="AE33" s="68"/>
+      <c r="AF33" s="68"/>
+      <c r="AG33" s="68"/>
+      <c r="AH33" s="68"/>
+      <c r="AI33" s="68"/>
+      <c r="AJ33" s="68"/>
+      <c r="AK33" s="68"/>
+      <c r="AL33" s="68"/>
+      <c r="AM33" s="68"/>
+      <c r="AN33" s="68"/>
+      <c r="AO33" s="68"/>
+      <c r="AP33" s="68"/>
+      <c r="AQ33" s="68"/>
+      <c r="AR33" s="68"/>
+      <c r="AS33" s="47"/>
     </row>
     <row r="34" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="100" t="s">
-        <v>19</v>
-      </c>
-      <c r="C34" s="81" t="s">
-        <v>49</v>
+      <c r="B34" s="114" t="s">
+        <v>53</v>
+      </c>
+      <c r="C34" s="113" t="s">
+        <v>55</v>
       </c>
       <c r="D34" s="7" t="s">
         <v>7</v>
@@ -3149,9 +3350,9 @@
       <c r="S34" s="17"/>
       <c r="T34" s="17"/>
       <c r="U34" s="21"/>
-      <c r="V34" s="55"/>
+      <c r="V34" s="54"/>
       <c r="W34" s="17"/>
-      <c r="X34" s="54"/>
+      <c r="X34" s="53"/>
       <c r="Y34" s="21"/>
       <c r="Z34" s="32"/>
       <c r="AA34" s="17"/>
@@ -3175,12 +3376,14 @@
       <c r="AS34" s="21"/>
     </row>
     <row r="35" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="100"/>
-      <c r="C35" s="81"/>
+      <c r="B35" s="114"/>
+      <c r="C35" s="113"/>
       <c r="D35" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E35" s="60"/>
+      <c r="E35" s="59">
+        <v>1.5</v>
+      </c>
       <c r="F35" s="14"/>
       <c r="G35" s="12"/>
       <c r="H35" s="12"/>
@@ -3199,8 +3402,8 @@
       <c r="U35" s="22"/>
       <c r="V35" s="33"/>
       <c r="W35" s="13"/>
-      <c r="X35" s="13"/>
-      <c r="Y35" s="22"/>
+      <c r="X35" s="76"/>
+      <c r="Y35" s="77"/>
       <c r="Z35" s="33"/>
       <c r="AA35" s="13"/>
       <c r="AB35" s="13"/>
@@ -3223,14 +3426,14 @@
       <c r="AS35" s="22"/>
     </row>
     <row r="36" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="100"/>
-      <c r="C36" s="98" t="s">
-        <v>50</v>
+      <c r="B36" s="114"/>
+      <c r="C36" s="120" t="s">
+        <v>48</v>
       </c>
       <c r="D36" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E36" s="65">
+      <c r="E36" s="64">
         <v>4</v>
       </c>
       <c r="F36" s="14"/>
@@ -3250,8 +3453,8 @@
       <c r="T36" s="13"/>
       <c r="U36" s="22"/>
       <c r="V36" s="33"/>
-      <c r="W36" s="51"/>
-      <c r="X36" s="51"/>
+      <c r="W36" s="50"/>
+      <c r="X36" s="50"/>
       <c r="Y36" s="31"/>
       <c r="Z36" s="42"/>
       <c r="AA36" s="13"/>
@@ -3275,12 +3478,12 @@
       <c r="AS36" s="22"/>
     </row>
     <row r="37" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="100"/>
-      <c r="C37" s="98"/>
+      <c r="B37" s="114"/>
+      <c r="C37" s="120"/>
       <c r="D37" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E37" s="60"/>
+      <c r="E37" s="59"/>
       <c r="F37" s="14"/>
       <c r="G37" s="12"/>
       <c r="H37" s="12"/>
@@ -3300,7 +3503,7 @@
       <c r="V37" s="33"/>
       <c r="W37" s="13"/>
       <c r="X37" s="13"/>
-      <c r="Y37" s="22"/>
+      <c r="Y37" s="77"/>
       <c r="Z37" s="33"/>
       <c r="AA37" s="13"/>
       <c r="AB37" s="13"/>
@@ -3323,15 +3526,15 @@
       <c r="AS37" s="22"/>
     </row>
     <row r="38" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="100"/>
-      <c r="C38" s="81" t="s">
-        <v>20</v>
+      <c r="B38" s="114"/>
+      <c r="C38" s="113" t="s">
+        <v>56</v>
       </c>
       <c r="D38" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E38" s="65">
-        <v>4</v>
+      <c r="E38" s="64">
+        <v>2</v>
       </c>
       <c r="F38" s="14"/>
       <c r="G38" s="12"/>
@@ -3352,10 +3555,10 @@
       <c r="V38" s="33"/>
       <c r="W38" s="13"/>
       <c r="X38" s="13"/>
-      <c r="Y38" s="53"/>
-      <c r="Z38" s="50"/>
+      <c r="Y38" s="52"/>
+      <c r="Z38" s="49"/>
       <c r="AA38" s="30"/>
-      <c r="AB38" s="30"/>
+      <c r="AB38" s="50"/>
       <c r="AC38" s="22"/>
       <c r="AD38" s="33"/>
       <c r="AE38" s="13"/>
@@ -3375,12 +3578,12 @@
       <c r="AS38" s="22"/>
     </row>
     <row r="39" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="100"/>
-      <c r="C39" s="81"/>
+      <c r="B39" s="114"/>
+      <c r="C39" s="113"/>
       <c r="D39" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E39" s="60"/>
+      <c r="E39" s="59"/>
       <c r="F39" s="14"/>
       <c r="G39" s="12"/>
       <c r="H39" s="12"/>
@@ -3423,9 +3626,9 @@
       <c r="AS39" s="22"/>
     </row>
     <row r="40" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="100"/>
-      <c r="C40" s="81" t="s">
-        <v>21</v>
+      <c r="B40" s="114"/>
+      <c r="C40" s="113" t="s">
+        <v>20</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>7</v>
@@ -3454,9 +3657,9 @@
       <c r="X40" s="13"/>
       <c r="Y40" s="22"/>
       <c r="Z40" s="33"/>
-      <c r="AA40" s="51"/>
-      <c r="AB40" s="13"/>
-      <c r="AC40" s="31"/>
+      <c r="AA40" s="50"/>
+      <c r="AB40" s="30"/>
+      <c r="AC40" s="52"/>
       <c r="AD40" s="33"/>
       <c r="AE40" s="13"/>
       <c r="AF40" s="13"/>
@@ -3475,12 +3678,12 @@
       <c r="AS40" s="22"/>
     </row>
     <row r="41" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="101"/>
-      <c r="C41" s="82"/>
+      <c r="B41" s="118"/>
+      <c r="C41" s="116"/>
       <c r="D41" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E41" s="63"/>
+      <c r="E41" s="62"/>
       <c r="F41" s="18"/>
       <c r="G41" s="19"/>
       <c r="H41" s="19"/>
@@ -3523,66 +3726,66 @@
       <c r="AS41" s="23"/>
     </row>
     <row r="42" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="99" t="s">
+      <c r="B42" s="117" t="s">
+        <v>21</v>
+      </c>
+      <c r="C42" s="115" t="s">
         <v>22</v>
-      </c>
-      <c r="C42" s="102" t="s">
-        <v>23</v>
       </c>
       <c r="D42" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E42" s="64">
-        <v>10</v>
-      </c>
-      <c r="F42" s="24"/>
-      <c r="G42" s="25"/>
-      <c r="H42" s="25"/>
-      <c r="I42" s="41"/>
-      <c r="J42" s="36"/>
-      <c r="K42" s="26"/>
-      <c r="L42" s="26"/>
-      <c r="M42" s="27"/>
-      <c r="N42" s="36"/>
-      <c r="O42" s="26"/>
-      <c r="P42" s="26"/>
-      <c r="Q42" s="27"/>
-      <c r="R42" s="36"/>
-      <c r="S42" s="26"/>
-      <c r="T42" s="26"/>
-      <c r="U42" s="27"/>
-      <c r="V42" s="36"/>
-      <c r="W42" s="26"/>
-      <c r="X42" s="26"/>
-      <c r="Y42" s="27"/>
-      <c r="Z42" s="36"/>
-      <c r="AA42" s="26"/>
-      <c r="AB42" s="56"/>
-      <c r="AC42" s="52"/>
-      <c r="AD42" s="35"/>
-      <c r="AE42" s="29"/>
-      <c r="AF42" s="29"/>
-      <c r="AG42" s="43"/>
-      <c r="AH42" s="35"/>
-      <c r="AI42" s="26"/>
-      <c r="AJ42" s="26"/>
-      <c r="AK42" s="27"/>
-      <c r="AL42" s="36"/>
-      <c r="AM42" s="26"/>
-      <c r="AN42" s="26"/>
-      <c r="AO42" s="27"/>
-      <c r="AP42" s="36"/>
-      <c r="AQ42" s="26"/>
-      <c r="AR42" s="26"/>
-      <c r="AS42" s="27"/>
+      <c r="E42" s="63">
+        <v>8</v>
+      </c>
+      <c r="F42" s="15"/>
+      <c r="G42" s="16"/>
+      <c r="H42" s="16"/>
+      <c r="I42" s="37"/>
+      <c r="J42" s="32"/>
+      <c r="K42" s="17"/>
+      <c r="L42" s="17"/>
+      <c r="M42" s="21"/>
+      <c r="N42" s="32"/>
+      <c r="O42" s="17"/>
+      <c r="P42" s="17"/>
+      <c r="Q42" s="21"/>
+      <c r="R42" s="32"/>
+      <c r="S42" s="17"/>
+      <c r="T42" s="17"/>
+      <c r="U42" s="21"/>
+      <c r="V42" s="32"/>
+      <c r="W42" s="17"/>
+      <c r="X42" s="17"/>
+      <c r="Y42" s="21"/>
+      <c r="Z42" s="32"/>
+      <c r="AA42" s="17"/>
+      <c r="AB42" s="97"/>
+      <c r="AC42" s="100"/>
+      <c r="AD42" s="99"/>
+      <c r="AE42" s="53"/>
+      <c r="AF42" s="53"/>
+      <c r="AG42" s="98"/>
+      <c r="AH42" s="54"/>
+      <c r="AI42" s="17"/>
+      <c r="AJ42" s="17"/>
+      <c r="AK42" s="21"/>
+      <c r="AL42" s="32"/>
+      <c r="AM42" s="17"/>
+      <c r="AN42" s="17"/>
+      <c r="AO42" s="21"/>
+      <c r="AP42" s="32"/>
+      <c r="AQ42" s="17"/>
+      <c r="AR42" s="17"/>
+      <c r="AS42" s="21"/>
     </row>
     <row r="43" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="100"/>
-      <c r="C43" s="81"/>
+      <c r="B43" s="114"/>
+      <c r="C43" s="113"/>
       <c r="D43" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E43" s="60"/>
+      <c r="E43" s="59"/>
       <c r="F43" s="14"/>
       <c r="G43" s="12"/>
       <c r="H43" s="12"/>
@@ -3625,14 +3828,14 @@
       <c r="AS43" s="22"/>
     </row>
     <row r="44" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="100"/>
-      <c r="C44" s="81" t="s">
-        <v>24</v>
+      <c r="B44" s="114"/>
+      <c r="C44" s="113" t="s">
+        <v>23</v>
       </c>
       <c r="D44" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E44" s="65">
+      <c r="E44" s="64">
         <v>10</v>
       </c>
       <c r="F44" s="14"/>
@@ -3662,27 +3865,27 @@
       <c r="AD44" s="33"/>
       <c r="AE44" s="13"/>
       <c r="AF44" s="13"/>
-      <c r="AG44" s="22"/>
-      <c r="AH44" s="50"/>
+      <c r="AG44" s="31"/>
+      <c r="AH44" s="42"/>
       <c r="AI44" s="30"/>
       <c r="AJ44" s="30"/>
       <c r="AK44" s="31"/>
-      <c r="AL44" s="42"/>
-      <c r="AM44" s="30"/>
-      <c r="AN44" s="13"/>
-      <c r="AO44" s="22"/>
-      <c r="AP44" s="33"/>
-      <c r="AQ44" s="13"/>
-      <c r="AR44" s="13"/>
-      <c r="AS44" s="22"/>
+      <c r="AL44" s="49"/>
+      <c r="AM44" s="50"/>
+      <c r="AN44" s="50"/>
+      <c r="AO44" s="52"/>
+      <c r="AP44" s="49"/>
+      <c r="AQ44" s="50"/>
+      <c r="AR44" s="50"/>
+      <c r="AS44" s="52"/>
     </row>
     <row r="45" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="100"/>
-      <c r="C45" s="81"/>
+      <c r="B45" s="114"/>
+      <c r="C45" s="113"/>
       <c r="D45" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E45" s="60"/>
+      <c r="E45" s="59"/>
       <c r="F45" s="14"/>
       <c r="G45" s="12"/>
       <c r="H45" s="12"/>
@@ -3715,25 +3918,25 @@
       <c r="AI45" s="13"/>
       <c r="AJ45" s="13"/>
       <c r="AK45" s="22"/>
-      <c r="AL45" s="33"/>
-      <c r="AM45" s="13"/>
-      <c r="AN45" s="13"/>
-      <c r="AO45" s="22"/>
-      <c r="AP45" s="33"/>
-      <c r="AQ45" s="13"/>
-      <c r="AR45" s="13"/>
-      <c r="AS45" s="22"/>
+      <c r="AL45" s="49"/>
+      <c r="AM45" s="50"/>
+      <c r="AN45" s="50"/>
+      <c r="AO45" s="52"/>
+      <c r="AP45" s="49"/>
+      <c r="AQ45" s="50"/>
+      <c r="AR45" s="50"/>
+      <c r="AS45" s="52"/>
     </row>
     <row r="46" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="100"/>
-      <c r="C46" s="81" t="s">
-        <v>51</v>
-      </c>
-      <c r="D46" s="4" t="s">
+      <c r="B46" s="114"/>
+      <c r="C46" s="113" t="s">
+        <v>49</v>
+      </c>
+      <c r="D46" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E46" s="2">
-        <v>4</v>
+      <c r="E46" s="60">
+        <v>2</v>
       </c>
       <c r="F46" s="14"/>
       <c r="G46" s="12"/>
@@ -3767,22 +3970,22 @@
       <c r="AI46" s="13"/>
       <c r="AJ46" s="13"/>
       <c r="AK46" s="22"/>
-      <c r="AL46" s="33"/>
-      <c r="AM46" s="13"/>
-      <c r="AN46" s="30"/>
-      <c r="AO46" s="31"/>
-      <c r="AP46" s="33"/>
-      <c r="AQ46" s="13"/>
-      <c r="AR46" s="13"/>
-      <c r="AS46" s="22"/>
+      <c r="AL46" s="42"/>
+      <c r="AM46" s="50"/>
+      <c r="AN46" s="50"/>
+      <c r="AO46" s="52"/>
+      <c r="AP46" s="49"/>
+      <c r="AQ46" s="50"/>
+      <c r="AR46" s="50"/>
+      <c r="AS46" s="52"/>
     </row>
     <row r="47" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="101"/>
-      <c r="C47" s="82"/>
+      <c r="B47" s="118"/>
+      <c r="C47" s="116"/>
       <c r="D47" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E47" s="63"/>
+      <c r="E47" s="62"/>
       <c r="F47" s="18"/>
       <c r="G47" s="19"/>
       <c r="H47" s="19"/>
@@ -3815,176 +4018,176 @@
       <c r="AI47" s="20"/>
       <c r="AJ47" s="20"/>
       <c r="AK47" s="23"/>
-      <c r="AL47" s="34"/>
-      <c r="AM47" s="20"/>
-      <c r="AN47" s="20"/>
-      <c r="AO47" s="23"/>
-      <c r="AP47" s="34"/>
-      <c r="AQ47" s="20"/>
-      <c r="AR47" s="20"/>
-      <c r="AS47" s="23"/>
+      <c r="AL47" s="105"/>
+      <c r="AM47" s="103"/>
+      <c r="AN47" s="103"/>
+      <c r="AO47" s="104"/>
+      <c r="AP47" s="105"/>
+      <c r="AQ47" s="103"/>
+      <c r="AR47" s="103"/>
+      <c r="AS47" s="104"/>
     </row>
     <row r="48" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="99" t="s">
-        <v>18</v>
-      </c>
-      <c r="C48" s="102" t="s">
-        <v>25</v>
+      <c r="B48" s="114" t="s">
+        <v>52</v>
+      </c>
+      <c r="C48" s="115" t="s">
+        <v>54</v>
       </c>
       <c r="D48" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E48" s="64">
-        <v>6</v>
-      </c>
-      <c r="F48" s="24"/>
-      <c r="G48" s="25"/>
-      <c r="H48" s="25"/>
-      <c r="I48" s="41"/>
-      <c r="J48" s="36"/>
-      <c r="K48" s="26"/>
-      <c r="L48" s="26"/>
-      <c r="M48" s="27"/>
-      <c r="N48" s="36"/>
-      <c r="O48" s="26"/>
-      <c r="P48" s="26"/>
-      <c r="Q48" s="27"/>
-      <c r="R48" s="36"/>
-      <c r="S48" s="26"/>
-      <c r="T48" s="26"/>
-      <c r="U48" s="27"/>
-      <c r="V48" s="36"/>
-      <c r="W48" s="26"/>
-      <c r="X48" s="26"/>
-      <c r="Y48" s="27"/>
-      <c r="Z48" s="36"/>
-      <c r="AA48" s="26"/>
-      <c r="AB48" s="26"/>
-      <c r="AC48" s="27"/>
-      <c r="AD48" s="36"/>
-      <c r="AE48" s="26"/>
-      <c r="AF48" s="26"/>
-      <c r="AG48" s="27"/>
-      <c r="AH48" s="36"/>
-      <c r="AI48" s="26"/>
-      <c r="AJ48" s="26"/>
-      <c r="AK48" s="27"/>
-      <c r="AL48" s="36"/>
-      <c r="AM48" s="26"/>
-      <c r="AN48" s="26"/>
-      <c r="AO48" s="27"/>
-      <c r="AP48" s="35"/>
-      <c r="AQ48" s="29"/>
-      <c r="AR48" s="29"/>
-      <c r="AS48" s="27"/>
+      <c r="E48" s="2">
+        <v>2</v>
+      </c>
+      <c r="F48" s="90"/>
+      <c r="G48" s="91"/>
+      <c r="H48" s="91"/>
+      <c r="I48" s="92"/>
+      <c r="J48" s="93"/>
+      <c r="K48" s="94"/>
+      <c r="L48" s="94"/>
+      <c r="M48" s="95"/>
+      <c r="N48" s="93"/>
+      <c r="O48" s="94"/>
+      <c r="P48" s="94"/>
+      <c r="Q48" s="95"/>
+      <c r="R48" s="93"/>
+      <c r="S48" s="94"/>
+      <c r="T48" s="94"/>
+      <c r="U48" s="95"/>
+      <c r="V48" s="93"/>
+      <c r="W48" s="94"/>
+      <c r="X48" s="94"/>
+      <c r="Y48" s="95"/>
+      <c r="Z48" s="93"/>
+      <c r="AA48" s="94"/>
+      <c r="AB48" s="94"/>
+      <c r="AC48" s="95"/>
+      <c r="AD48" s="93"/>
+      <c r="AE48" s="94"/>
+      <c r="AF48" s="94"/>
+      <c r="AG48" s="95"/>
+      <c r="AH48" s="93"/>
+      <c r="AI48" s="94"/>
+      <c r="AJ48" s="94"/>
+      <c r="AK48" s="95"/>
+      <c r="AL48" s="108"/>
+      <c r="AM48" s="96"/>
+      <c r="AN48" s="106"/>
+      <c r="AO48" s="107"/>
+      <c r="AP48" s="108"/>
+      <c r="AQ48" s="106"/>
+      <c r="AR48" s="106"/>
+      <c r="AS48" s="107"/>
     </row>
     <row r="49" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="100"/>
-      <c r="C49" s="81"/>
+      <c r="B49" s="114"/>
+      <c r="C49" s="113"/>
       <c r="D49" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E49" s="60"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="12"/>
-      <c r="H49" s="12"/>
-      <c r="I49" s="38"/>
-      <c r="J49" s="33"/>
-      <c r="K49" s="13"/>
-      <c r="L49" s="13"/>
-      <c r="M49" s="22"/>
-      <c r="N49" s="33"/>
-      <c r="O49" s="13"/>
-      <c r="P49" s="13"/>
-      <c r="Q49" s="22"/>
-      <c r="R49" s="33"/>
-      <c r="S49" s="13"/>
-      <c r="T49" s="13"/>
-      <c r="U49" s="22"/>
-      <c r="V49" s="33"/>
-      <c r="W49" s="13"/>
-      <c r="X49" s="13"/>
-      <c r="Y49" s="22"/>
-      <c r="Z49" s="33"/>
-      <c r="AA49" s="13"/>
-      <c r="AB49" s="13"/>
-      <c r="AC49" s="22"/>
-      <c r="AD49" s="33"/>
-      <c r="AE49" s="13"/>
-      <c r="AF49" s="13"/>
-      <c r="AG49" s="22"/>
-      <c r="AH49" s="33"/>
-      <c r="AI49" s="13"/>
-      <c r="AJ49" s="13"/>
-      <c r="AK49" s="22"/>
-      <c r="AL49" s="33"/>
-      <c r="AM49" s="13"/>
-      <c r="AN49" s="13"/>
-      <c r="AO49" s="22"/>
-      <c r="AP49" s="33"/>
-      <c r="AQ49" s="13"/>
-      <c r="AR49" s="13"/>
-      <c r="AS49" s="22"/>
+      <c r="E49" s="61"/>
+      <c r="F49" s="82"/>
+      <c r="G49" s="83"/>
+      <c r="H49" s="83"/>
+      <c r="I49" s="84"/>
+      <c r="J49" s="85"/>
+      <c r="K49" s="86"/>
+      <c r="L49" s="86"/>
+      <c r="M49" s="87"/>
+      <c r="N49" s="85"/>
+      <c r="O49" s="86"/>
+      <c r="P49" s="86"/>
+      <c r="Q49" s="87"/>
+      <c r="R49" s="85"/>
+      <c r="S49" s="86"/>
+      <c r="T49" s="86"/>
+      <c r="U49" s="87"/>
+      <c r="V49" s="85"/>
+      <c r="W49" s="86"/>
+      <c r="X49" s="86"/>
+      <c r="Y49" s="87"/>
+      <c r="Z49" s="85"/>
+      <c r="AA49" s="86"/>
+      <c r="AB49" s="86"/>
+      <c r="AC49" s="87"/>
+      <c r="AD49" s="85"/>
+      <c r="AE49" s="86"/>
+      <c r="AF49" s="86"/>
+      <c r="AG49" s="87"/>
+      <c r="AH49" s="85"/>
+      <c r="AI49" s="86"/>
+      <c r="AJ49" s="86"/>
+      <c r="AK49" s="87"/>
+      <c r="AL49" s="109"/>
+      <c r="AM49" s="101"/>
+      <c r="AN49" s="101"/>
+      <c r="AO49" s="102"/>
+      <c r="AP49" s="109"/>
+      <c r="AQ49" s="101"/>
+      <c r="AR49" s="101"/>
+      <c r="AS49" s="102"/>
     </row>
     <row r="50" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="100"/>
-      <c r="C50" s="81" t="s">
-        <v>21</v>
-      </c>
-      <c r="D50" s="4" t="s">
+      <c r="B50" s="114"/>
+      <c r="C50" s="113" t="s">
+        <v>19</v>
+      </c>
+      <c r="D50" s="7" t="s">
         <v>7</v>
       </c>
       <c r="E50" s="2">
-        <v>2</v>
-      </c>
-      <c r="F50" s="14"/>
-      <c r="G50" s="12"/>
-      <c r="H50" s="12"/>
-      <c r="I50" s="38"/>
-      <c r="J50" s="33"/>
-      <c r="K50" s="13"/>
-      <c r="L50" s="13"/>
-      <c r="M50" s="22"/>
-      <c r="N50" s="33"/>
-      <c r="O50" s="13"/>
-      <c r="P50" s="13"/>
-      <c r="Q50" s="22"/>
-      <c r="R50" s="33"/>
-      <c r="S50" s="13"/>
-      <c r="T50" s="13"/>
-      <c r="U50" s="22"/>
-      <c r="V50" s="33"/>
-      <c r="W50" s="13"/>
-      <c r="X50" s="13"/>
-      <c r="Y50" s="22"/>
-      <c r="Z50" s="33"/>
-      <c r="AA50" s="13"/>
-      <c r="AB50" s="13"/>
-      <c r="AC50" s="22"/>
-      <c r="AD50" s="33"/>
-      <c r="AE50" s="13"/>
-      <c r="AF50" s="13"/>
-      <c r="AG50" s="22"/>
-      <c r="AH50" s="33"/>
-      <c r="AI50" s="13"/>
-      <c r="AJ50" s="13"/>
-      <c r="AK50" s="22"/>
-      <c r="AL50" s="33"/>
-      <c r="AM50" s="13"/>
-      <c r="AN50" s="13"/>
-      <c r="AO50" s="22"/>
-      <c r="AP50" s="33"/>
-      <c r="AQ50" s="13"/>
-      <c r="AR50" s="13"/>
-      <c r="AS50" s="31"/>
+        <v>4</v>
+      </c>
+      <c r="F50" s="82"/>
+      <c r="G50" s="83"/>
+      <c r="H50" s="83"/>
+      <c r="I50" s="84"/>
+      <c r="J50" s="85"/>
+      <c r="K50" s="86"/>
+      <c r="L50" s="86"/>
+      <c r="M50" s="87"/>
+      <c r="N50" s="85"/>
+      <c r="O50" s="86"/>
+      <c r="P50" s="86"/>
+      <c r="Q50" s="87"/>
+      <c r="R50" s="85"/>
+      <c r="S50" s="86"/>
+      <c r="T50" s="86"/>
+      <c r="U50" s="87"/>
+      <c r="V50" s="85"/>
+      <c r="W50" s="86"/>
+      <c r="X50" s="86"/>
+      <c r="Y50" s="87"/>
+      <c r="Z50" s="85"/>
+      <c r="AA50" s="86"/>
+      <c r="AB50" s="86"/>
+      <c r="AC50" s="87"/>
+      <c r="AD50" s="85"/>
+      <c r="AE50" s="86"/>
+      <c r="AF50" s="86"/>
+      <c r="AG50" s="87"/>
+      <c r="AH50" s="85"/>
+      <c r="AI50" s="86"/>
+      <c r="AJ50" s="86"/>
+      <c r="AK50" s="87"/>
+      <c r="AL50" s="109"/>
+      <c r="AM50" s="101"/>
+      <c r="AN50" s="88"/>
+      <c r="AO50" s="89"/>
+      <c r="AP50" s="109"/>
+      <c r="AQ50" s="101"/>
+      <c r="AR50" s="101"/>
+      <c r="AS50" s="102"/>
     </row>
     <row r="51" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="101"/>
-      <c r="C51" s="82"/>
-      <c r="D51" s="5" t="s">
+      <c r="B51" s="118"/>
+      <c r="C51" s="116"/>
+      <c r="D51" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E51" s="6"/>
+      <c r="E51" s="62"/>
       <c r="F51" s="18"/>
       <c r="G51" s="19"/>
       <c r="H51" s="19"/>
@@ -4017,44 +4220,236 @@
       <c r="AI51" s="20"/>
       <c r="AJ51" s="20"/>
       <c r="AK51" s="23"/>
-      <c r="AL51" s="34"/>
-      <c r="AM51" s="20"/>
-      <c r="AN51" s="20"/>
-      <c r="AO51" s="23"/>
-      <c r="AP51" s="34"/>
-      <c r="AQ51" s="20"/>
-      <c r="AR51" s="20"/>
-      <c r="AS51" s="23"/>
+      <c r="AL51" s="105"/>
+      <c r="AM51" s="103"/>
+      <c r="AN51" s="103"/>
+      <c r="AO51" s="104"/>
+      <c r="AP51" s="105"/>
+      <c r="AQ51" s="103"/>
+      <c r="AR51" s="103"/>
+      <c r="AS51" s="104"/>
+    </row>
+    <row r="52" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="117" t="s">
+        <v>18</v>
+      </c>
+      <c r="C52" s="115" t="s">
+        <v>24</v>
+      </c>
+      <c r="D52" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E52" s="63">
+        <v>4</v>
+      </c>
+      <c r="F52" s="24"/>
+      <c r="G52" s="25"/>
+      <c r="H52" s="25"/>
+      <c r="I52" s="41"/>
+      <c r="J52" s="36"/>
+      <c r="K52" s="26"/>
+      <c r="L52" s="26"/>
+      <c r="M52" s="27"/>
+      <c r="N52" s="36"/>
+      <c r="O52" s="26"/>
+      <c r="P52" s="26"/>
+      <c r="Q52" s="27"/>
+      <c r="R52" s="36"/>
+      <c r="S52" s="26"/>
+      <c r="T52" s="26"/>
+      <c r="U52" s="27"/>
+      <c r="V52" s="36"/>
+      <c r="W52" s="26"/>
+      <c r="X52" s="26"/>
+      <c r="Y52" s="27"/>
+      <c r="Z52" s="36"/>
+      <c r="AA52" s="26"/>
+      <c r="AB52" s="26"/>
+      <c r="AC52" s="27"/>
+      <c r="AD52" s="36"/>
+      <c r="AE52" s="26"/>
+      <c r="AF52" s="26"/>
+      <c r="AG52" s="27"/>
+      <c r="AH52" s="36"/>
+      <c r="AI52" s="26"/>
+      <c r="AJ52" s="26"/>
+      <c r="AK52" s="27"/>
+      <c r="AL52" s="110"/>
+      <c r="AM52" s="55"/>
+      <c r="AN52" s="55"/>
+      <c r="AO52" s="51"/>
+      <c r="AP52" s="35"/>
+      <c r="AQ52" s="29"/>
+      <c r="AR52" s="55"/>
+      <c r="AS52" s="51"/>
+    </row>
+    <row r="53" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="114"/>
+      <c r="C53" s="113"/>
+      <c r="D53" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E53" s="59"/>
+      <c r="F53" s="14"/>
+      <c r="G53" s="12"/>
+      <c r="H53" s="12"/>
+      <c r="I53" s="38"/>
+      <c r="J53" s="33"/>
+      <c r="K53" s="13"/>
+      <c r="L53" s="13"/>
+      <c r="M53" s="22"/>
+      <c r="N53" s="33"/>
+      <c r="O53" s="13"/>
+      <c r="P53" s="13"/>
+      <c r="Q53" s="22"/>
+      <c r="R53" s="33"/>
+      <c r="S53" s="13"/>
+      <c r="T53" s="13"/>
+      <c r="U53" s="22"/>
+      <c r="V53" s="33"/>
+      <c r="W53" s="13"/>
+      <c r="X53" s="13"/>
+      <c r="Y53" s="22"/>
+      <c r="Z53" s="33"/>
+      <c r="AA53" s="13"/>
+      <c r="AB53" s="13"/>
+      <c r="AC53" s="22"/>
+      <c r="AD53" s="33"/>
+      <c r="AE53" s="13"/>
+      <c r="AF53" s="13"/>
+      <c r="AG53" s="22"/>
+      <c r="AH53" s="33"/>
+      <c r="AI53" s="13"/>
+      <c r="AJ53" s="13"/>
+      <c r="AK53" s="22"/>
+      <c r="AL53" s="49"/>
+      <c r="AM53" s="50"/>
+      <c r="AN53" s="50"/>
+      <c r="AO53" s="52"/>
+      <c r="AP53" s="49"/>
+      <c r="AQ53" s="50"/>
+      <c r="AR53" s="50"/>
+      <c r="AS53" s="52"/>
+    </row>
+    <row r="54" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="114"/>
+      <c r="C54" s="113" t="s">
+        <v>20</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E54" s="2">
+        <v>4</v>
+      </c>
+      <c r="F54" s="14"/>
+      <c r="G54" s="12"/>
+      <c r="H54" s="12"/>
+      <c r="I54" s="38"/>
+      <c r="J54" s="33"/>
+      <c r="K54" s="13"/>
+      <c r="L54" s="13"/>
+      <c r="M54" s="22"/>
+      <c r="N54" s="33"/>
+      <c r="O54" s="13"/>
+      <c r="P54" s="13"/>
+      <c r="Q54" s="22"/>
+      <c r="R54" s="33"/>
+      <c r="S54" s="13"/>
+      <c r="T54" s="13"/>
+      <c r="U54" s="22"/>
+      <c r="V54" s="33"/>
+      <c r="W54" s="13"/>
+      <c r="X54" s="13"/>
+      <c r="Y54" s="22"/>
+      <c r="Z54" s="33"/>
+      <c r="AA54" s="13"/>
+      <c r="AB54" s="13"/>
+      <c r="AC54" s="22"/>
+      <c r="AD54" s="33"/>
+      <c r="AE54" s="13"/>
+      <c r="AF54" s="13"/>
+      <c r="AG54" s="22"/>
+      <c r="AH54" s="33"/>
+      <c r="AI54" s="13"/>
+      <c r="AJ54" s="13"/>
+      <c r="AK54" s="22"/>
+      <c r="AL54" s="49"/>
+      <c r="AM54" s="50"/>
+      <c r="AN54" s="50"/>
+      <c r="AO54" s="52"/>
+      <c r="AP54" s="49"/>
+      <c r="AQ54" s="50"/>
+      <c r="AR54" s="30"/>
+      <c r="AS54" s="31"/>
+    </row>
+    <row r="55" spans="2:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="118"/>
+      <c r="C55" s="116"/>
+      <c r="D55" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E55" s="6"/>
+      <c r="F55" s="18"/>
+      <c r="G55" s="19"/>
+      <c r="H55" s="19"/>
+      <c r="I55" s="40"/>
+      <c r="J55" s="34"/>
+      <c r="K55" s="20"/>
+      <c r="L55" s="20"/>
+      <c r="M55" s="23"/>
+      <c r="N55" s="34"/>
+      <c r="O55" s="20"/>
+      <c r="P55" s="20"/>
+      <c r="Q55" s="23"/>
+      <c r="R55" s="34"/>
+      <c r="S55" s="20"/>
+      <c r="T55" s="20"/>
+      <c r="U55" s="23"/>
+      <c r="V55" s="34"/>
+      <c r="W55" s="20"/>
+      <c r="X55" s="20"/>
+      <c r="Y55" s="23"/>
+      <c r="Z55" s="34"/>
+      <c r="AA55" s="20"/>
+      <c r="AB55" s="20"/>
+      <c r="AC55" s="23"/>
+      <c r="AD55" s="34"/>
+      <c r="AE55" s="20"/>
+      <c r="AF55" s="20"/>
+      <c r="AG55" s="23"/>
+      <c r="AH55" s="34"/>
+      <c r="AI55" s="20"/>
+      <c r="AJ55" s="20"/>
+      <c r="AK55" s="23"/>
+      <c r="AL55" s="34"/>
+      <c r="AM55" s="20"/>
+      <c r="AN55" s="20"/>
+      <c r="AO55" s="23"/>
+      <c r="AP55" s="34"/>
+      <c r="AQ55" s="20"/>
+      <c r="AR55" s="20"/>
+      <c r="AS55" s="23"/>
     </row>
   </sheetData>
-  <mergeCells count="57">
-    <mergeCell ref="G8:W8"/>
-    <mergeCell ref="X32:AS32"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="B28:B31"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="C16:C17"/>
+  <mergeCells count="60">
+    <mergeCell ref="F8:V8"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
     <mergeCell ref="B10:B15"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="B16:B27"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="C24:C25"/>
     <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="B48:B51"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="B42:B47"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="B34:B41"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="R3:U3"/>
+    <mergeCell ref="R4:U4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B3:C4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="D3:E4"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="J4:M4"/>
     <mergeCell ref="B2:AS2"/>
     <mergeCell ref="AP3:AS3"/>
     <mergeCell ref="Z4:AC4"/>
@@ -4071,20 +4466,33 @@
     <mergeCell ref="J3:M3"/>
     <mergeCell ref="N3:Q3"/>
     <mergeCell ref="N4:Q4"/>
-    <mergeCell ref="R3:U3"/>
-    <mergeCell ref="R4:U4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B3:C4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="D3:E4"/>
-    <mergeCell ref="F4:I4"/>
-    <mergeCell ref="J4:M4"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="B52:B55"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="B34:B41"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="B42:B47"/>
+    <mergeCell ref="B48:B51"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="X32:AS32"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="B28:B31"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="B16:B27"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="B32:B33"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="52" orientation="landscape" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>